<commit_message>
Updated JS 10.0 tagged interfaces & sample switch configs
</commit_message>
<xml_diff>
--- a/data/sample_switch_configs/Solution-Workbook.xlsx
+++ b/data/sample_switch_configs/Solution-Workbook.xlsx
@@ -5,12 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DTK-Updates\JS-10.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DTK-Updates\Updated fo JS-10.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="9j4ykewDrYAg2tL7w9G2lZB8TnHiu4FGNmBFcdNR5GaQjB3ocP4bWmmjMUgmpCfkML5FZZ3wTaRUkpONDK4x6w==" workbookSaltValue="Ty0wE88Qz37SCXXNbJS1cA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6760" tabRatio="782" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6760" tabRatio="782"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -8288,198 +8287,6 @@
   </cellStyles>
   <dxfs count="163">
     <dxf>
-      <fill>
-        <patternFill patternType="mediumGray"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="mediumGray"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="mediumGray"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="mediumGray"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="mediumGray"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="mediumGray"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="mediumGray"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="mediumGray"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="mediumGray"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="mediumGray"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="mediumGray"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="mediumGray"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="mediumGray"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="mediumGray"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="mediumGray"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="mediumGray"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="mediumGray"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -8494,6 +8301,19 @@
           <color rgb="FFFFFFFF"/>
         </top>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -8850,6 +8670,16 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray"/>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -9235,6 +9065,16 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray"/>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -9762,6 +9602,36 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="mediumGray"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray"/>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -9868,6 +9738,83 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -10087,6 +10034,58 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -10235,19 +10234,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>131722</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>196850</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>36510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="4" name="Picture 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -10267,8 +10266,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="76200" y="0"/>
-          <a:ext cx="7759700" cy="6399172"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="8121650" cy="6697660"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12257,187 +12256,187 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B4:E9" totalsRowShown="0" headerRowDxfId="162" dataDxfId="161">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B4:E9" totalsRowShown="0" headerRowDxfId="155" dataDxfId="154">
   <autoFilter ref="B4:E9"/>
   <sortState ref="B2:E120">
     <sortCondition ref="B1:B120"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" name="Dell Order#" dataDxfId="160"/>
-    <tableColumn id="2" name="SKU #" dataDxfId="159"/>
-    <tableColumn id="3" name="Description" dataDxfId="158"/>
-    <tableColumn id="4" name="Qty" dataDxfId="157"/>
+    <tableColumn id="1" name="Dell Order#" dataDxfId="153"/>
+    <tableColumn id="2" name="SKU #" dataDxfId="152"/>
+    <tableColumn id="3" name="Description" dataDxfId="151"/>
+    <tableColumn id="4" name="Qty" dataDxfId="150"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="144" name="Table144" displayName="Table144" ref="G3:G9" totalsRowShown="0" headerRowDxfId="128" dataDxfId="127">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="144" name="Table144" displayName="Table144" ref="G3:G9" totalsRowShown="0" headerRowDxfId="108" dataDxfId="107">
   <autoFilter ref="G3:G9"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Login Methods" dataDxfId="126"/>
+    <tableColumn id="1" name="Login Methods" dataDxfId="106"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="176" name="Table144177" displayName="Table144177" ref="I3:I8" totalsRowShown="0" headerRowDxfId="125" dataDxfId="124">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="176" name="Table144177" displayName="Table144177" ref="I3:I8" totalsRowShown="0" headerRowDxfId="105" dataDxfId="104">
   <autoFilter ref="I3:I8"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Enable Methods" dataDxfId="123"/>
+    <tableColumn id="1" name="Enable Methods" dataDxfId="103"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="177" name="Table144177178" displayName="Table144177178" ref="K3:K8" totalsRowShown="0" headerRowDxfId="122" dataDxfId="121">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="177" name="Table144177178" displayName="Table144177178" ref="K3:K8" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101">
   <autoFilter ref="K3:K8"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Exec Methods" dataDxfId="120"/>
+    <tableColumn id="1" name="Exec Methods" dataDxfId="100"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="178" name="Table144177178179" displayName="Table144177178179" ref="M3:M6" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="178" name="Table144177178179" displayName="Table144177178179" ref="M3:M6" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98">
   <autoFilter ref="M3:M6"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Commands Methods" dataDxfId="117"/>
+    <tableColumn id="1" name="Commands Methods" dataDxfId="97"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="179" name="Table144177178179180" displayName="Table144177178179180" ref="O3:O5" totalsRowShown="0" headerRowDxfId="116" dataDxfId="115">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="179" name="Table144177178179180" displayName="Table144177178179180" ref="O3:O5" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95">
   <autoFilter ref="O3:O5"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Config-Commands" dataDxfId="114"/>
+    <tableColumn id="1" name="Config-Commands" dataDxfId="94"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="188" name="Table144177178179180189" displayName="Table144177178179180189" ref="Q3:Q4" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="188" name="Table144177178179180189" displayName="Table144177178179180189" ref="Q3:Q4" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
   <autoFilter ref="Q3:Q4"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Accounting" dataDxfId="111"/>
+    <tableColumn id="1" name="Accounting" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="43" name="Table222144" displayName="Table222144" ref="E4:P57" totalsRowShown="0" headerRowDxfId="110" dataDxfId="109">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="43" name="Table222144" displayName="Table222144" ref="E4:P57" totalsRowShown="0" headerRowDxfId="84" dataDxfId="83">
   <autoFilter ref="E4:P57"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Name" dataDxfId="108"/>
-    <tableColumn id="5" name="Connector" dataDxfId="107"/>
-    <tableColumn id="2" name="Device Name" dataDxfId="106"/>
-    <tableColumn id="3" name="Port" dataDxfId="105"/>
-    <tableColumn id="4" name="Untagged" dataDxfId="104"/>
-    <tableColumn id="8" name="Tagged" dataDxfId="103"/>
-    <tableColumn id="11" name="Port State" dataDxfId="102"/>
-    <tableColumn id="10" name="STP Port Type" dataDxfId="101"/>
-    <tableColumn id="9" name="MTU" dataDxfId="100"/>
-    <tableColumn id="12" name="Flowcontrol" dataDxfId="99"/>
-    <tableColumn id="6" name="#" dataDxfId="98"/>
-    <tableColumn id="7" name="Mode" dataDxfId="97"/>
+    <tableColumn id="1" name="Name" dataDxfId="82"/>
+    <tableColumn id="5" name="Connector" dataDxfId="81"/>
+    <tableColumn id="2" name="Device Name" dataDxfId="80"/>
+    <tableColumn id="3" name="Port" dataDxfId="79"/>
+    <tableColumn id="4" name="Untagged" dataDxfId="78"/>
+    <tableColumn id="8" name="Tagged" dataDxfId="77"/>
+    <tableColumn id="11" name="Port State" dataDxfId="76"/>
+    <tableColumn id="10" name="STP Port Type" dataDxfId="75"/>
+    <tableColumn id="9" name="MTU" dataDxfId="74"/>
+    <tableColumn id="12" name="Flowcontrol" dataDxfId="73"/>
+    <tableColumn id="6" name="#" dataDxfId="72"/>
+    <tableColumn id="7" name="Mode" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table29521013" displayName="Table29521013" ref="A15:C23" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table29521013" displayName="Table29521013" ref="A15:C23" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69">
   <autoFilter ref="A15:C23"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Interface" dataDxfId="94"/>
-    <tableColumn id="2" name="IP /Netmask" dataDxfId="93"/>
-    <tableColumn id="3" name="Required?" dataDxfId="92"/>
+    <tableColumn id="1" name="Interface" dataDxfId="68"/>
+    <tableColumn id="2" name="IP /Netmask" dataDxfId="67"/>
+    <tableColumn id="3" name="Required?" dataDxfId="66"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table30531114" displayName="Table30531114" ref="A26:C29" totalsRowShown="0" headerRowDxfId="91" dataDxfId="90" tableBorderDxfId="89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table30531114" displayName="Table30531114" ref="A26:C29" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64" tableBorderDxfId="63">
   <autoFilter ref="A26:C29"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Destination" dataDxfId="88"/>
-    <tableColumn id="2" name="Next Hop" dataDxfId="87"/>
-    <tableColumn id="3" name="Required?" dataDxfId="86"/>
+    <tableColumn id="1" name="Destination" dataDxfId="62"/>
+    <tableColumn id="2" name="Next Hop" dataDxfId="61"/>
+    <tableColumn id="3" name="Required?" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table37591215" displayName="Table37591215" ref="A4:C13" totalsRowShown="0" headerRowDxfId="85" dataDxfId="84" tableBorderDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table37591215" displayName="Table37591215" ref="A4:C13" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58" tableBorderDxfId="57">
   <autoFilter ref="A4:C13"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="ID" dataDxfId="82"/>
-    <tableColumn id="2" name="Description" dataDxfId="81"/>
-    <tableColumn id="3" name="Required?" dataDxfId="80"/>
+    <tableColumn id="1" name="ID" dataDxfId="56"/>
+    <tableColumn id="2" name="Description" dataDxfId="55"/>
+    <tableColumn id="3" name="Required?" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="G4:G7" totalsRowShown="0" headerRowDxfId="156" dataDxfId="155">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="G4:G7" totalsRowShown="0" headerRowDxfId="149" dataDxfId="148">
   <autoFilter ref="G4:G7"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Legend" dataDxfId="154"/>
+    <tableColumn id="1" name="Legend" dataDxfId="147"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table22213210" displayName="Table22213210" ref="E3:Q58" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table22213210" displayName="Table22213210" ref="E3:Q58" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
   <autoFilter ref="E3:Q58"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="Name" dataDxfId="77"/>
-    <tableColumn id="5" name="Connector" dataDxfId="76"/>
-    <tableColumn id="2" name="Device Name" dataDxfId="75"/>
-    <tableColumn id="3" name="Port" dataDxfId="74"/>
-    <tableColumn id="4" name="Untagged" dataDxfId="73"/>
-    <tableColumn id="8" name="Tagged" dataDxfId="72"/>
+    <tableColumn id="1" name="Name" dataDxfId="49"/>
+    <tableColumn id="5" name="Connector" dataDxfId="48"/>
+    <tableColumn id="2" name="Device Name" dataDxfId="47"/>
+    <tableColumn id="3" name="Port" dataDxfId="46"/>
+    <tableColumn id="4" name="Untagged" dataDxfId="45"/>
+    <tableColumn id="8" name="Tagged" dataDxfId="44"/>
     <tableColumn id="9" name="Bond#"/>
     <tableColumn id="12" name="Port State"/>
     <tableColumn id="11" name="STP Port Type"/>
     <tableColumn id="13" name="MTU"/>
     <tableColumn id="10" name="Flow Control"/>
-    <tableColumn id="6" name="#" dataDxfId="71"/>
-    <tableColumn id="7" name="Mode" dataDxfId="70"/>
+    <tableColumn id="6" name="#" dataDxfId="43"/>
+    <tableColumn id="7" name="Mode" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table305311121820" displayName="Table305311121820" ref="A29:B32" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68" tableBorderDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table305311121820" displayName="Table305311121820" ref="A29:B32" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" tableBorderDxfId="39">
   <autoFilter ref="A29:B32"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Destination" dataDxfId="66"/>
-    <tableColumn id="2" name="Next Hop" dataDxfId="65"/>
+    <tableColumn id="1" name="Destination" dataDxfId="38"/>
+    <tableColumn id="2" name="Next Hop" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table2952101316171921" displayName="Table2952101316171921" ref="A16:B24" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table2952101316171921" displayName="Table2952101316171921" ref="A16:B24" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <autoFilter ref="A16:B24"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Interface" dataDxfId="62"/>
-    <tableColumn id="2" name="IP /Netmask" dataDxfId="61">
+    <tableColumn id="1" name="Interface" dataDxfId="34"/>
+    <tableColumn id="2" name="IP /Netmask" dataDxfId="33">
       <calculatedColumnFormula>S4048_1_OOB_IP</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -12446,56 +12445,56 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table3759121511" displayName="Table3759121511" ref="A4:C13" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59" tableBorderDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table3759121511" displayName="Table3759121511" ref="A4:C13" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" tableBorderDxfId="30">
   <autoFilter ref="A4:C13"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="ID" dataDxfId="57"/>
-    <tableColumn id="2" name="Description" dataDxfId="56"/>
-    <tableColumn id="3" name="Required?" dataDxfId="55"/>
+    <tableColumn id="1" name="ID" dataDxfId="29"/>
+    <tableColumn id="2" name="Description" dataDxfId="28"/>
+    <tableColumn id="3" name="Required?" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="Table222132" displayName="Table222132" ref="E4:Q59" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="Table222132" displayName="Table222132" ref="E4:Q59" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="E4:Q59"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="Name" dataDxfId="52"/>
-    <tableColumn id="5" name="Connector" dataDxfId="51"/>
-    <tableColumn id="2" name="Device Name" dataDxfId="50"/>
-    <tableColumn id="3" name="Port " dataDxfId="49"/>
-    <tableColumn id="4" name="Untagged" dataDxfId="48"/>
-    <tableColumn id="8" name="Tagged" dataDxfId="47"/>
+    <tableColumn id="1" name="Name" dataDxfId="22"/>
+    <tableColumn id="5" name="Connector" dataDxfId="21"/>
+    <tableColumn id="2" name="Device Name" dataDxfId="20"/>
+    <tableColumn id="3" name="Port " dataDxfId="19"/>
+    <tableColumn id="4" name="Untagged" dataDxfId="18"/>
+    <tableColumn id="8" name="Tagged" dataDxfId="17"/>
     <tableColumn id="9" name="Bond#"/>
     <tableColumn id="12" name="Port State"/>
     <tableColumn id="11" name="STP Port Type"/>
     <tableColumn id="13" name="MTU"/>
     <tableColumn id="10" name="Flow Control"/>
-    <tableColumn id="6" name="#" dataDxfId="46"/>
-    <tableColumn id="7" name="Mode" dataDxfId="45"/>
+    <tableColumn id="6" name="#" dataDxfId="16"/>
+    <tableColumn id="7" name="Mode" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table3053111218" displayName="Table3053111218" ref="A39:B42" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43" tableBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table3053111218" displayName="Table3053111218" ref="A39:B42" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
   <autoFilter ref="A39:B42"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Destination" dataDxfId="41"/>
-    <tableColumn id="2" name="Next Hop" dataDxfId="40"/>
+    <tableColumn id="1" name="Destination" dataDxfId="11"/>
+    <tableColumn id="2" name="Next Hop" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table29521013161719" displayName="Table29521013161719" ref="A15:B23" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table29521013161719" displayName="Table29521013161719" ref="A15:B23" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A15:B23"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Interface" dataDxfId="31"/>
-    <tableColumn id="2" name="IP /Netmask" dataDxfId="30">
+    <tableColumn id="1" name="Interface" dataDxfId="7"/>
+    <tableColumn id="2" name="IP /Netmask" dataDxfId="6">
       <calculatedColumnFormula>S4048_2_OOB_IP</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -12504,86 +12503,86 @@
 </file>
 
 <file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table3759121512" displayName="Table3759121512" ref="A4:C13" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" tableBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table3759121512" displayName="Table3759121512" ref="A4:C13" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="A4:C13"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="ID" dataDxfId="36"/>
-    <tableColumn id="2" name="Description" dataDxfId="35"/>
-    <tableColumn id="3" name="Required?" dataDxfId="34"/>
+    <tableColumn id="1" name="ID" dataDxfId="2"/>
+    <tableColumn id="2" name="Description" dataDxfId="1"/>
+    <tableColumn id="3" name="Required?" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Table2125" displayName="Table2125" ref="S3:W13" totalsRowShown="0" headerRowDxfId="153" dataDxfId="152">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Table2125" displayName="Table2125" ref="S3:W13" totalsRowShown="0" headerRowDxfId="146" dataDxfId="145">
   <autoFilter ref="S3:W13"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Network" dataDxfId="151"/>
-    <tableColumn id="2" name="SAH" dataDxfId="150"/>
-    <tableColumn id="3" name="OpenStack Controller" dataDxfId="149"/>
-    <tableColumn id="4" name="OpenStack Compute" dataDxfId="148"/>
-    <tableColumn id="5" name="Red Hat Ceph Storage" dataDxfId="147"/>
+    <tableColumn id="1" name="Network" dataDxfId="144"/>
+    <tableColumn id="2" name="SAH" dataDxfId="143"/>
+    <tableColumn id="3" name="OpenStack Controller" dataDxfId="142"/>
+    <tableColumn id="4" name="OpenStack Compute" dataDxfId="141"/>
+    <tableColumn id="5" name="Red Hat Ceph Storage" dataDxfId="140"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table6" displayName="Table6" ref="S3:S9" totalsRowShown="0" headerRowDxfId="146" dataDxfId="145">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table6" displayName="Table6" ref="S3:S9" totalsRowShown="0" headerRowDxfId="126" dataDxfId="125">
   <autoFilter ref="S3:S9"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Spanning-Tree Protocols" dataDxfId="144"/>
+    <tableColumn id="1" name="Spanning-Tree Protocols" dataDxfId="124"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table8" displayName="Table8" ref="U3:U20" totalsRowShown="0" headerRowDxfId="143" dataDxfId="142">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table8" displayName="Table8" ref="U3:U20" totalsRowShown="0" headerRowDxfId="123" dataDxfId="122">
   <autoFilter ref="U3:U20"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="STP Priorities" dataDxfId="141"/>
+    <tableColumn id="1" name="STP Priorities" dataDxfId="121"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table610" displayName="Table610" ref="W3:W8" totalsRowShown="0" headerRowDxfId="140" dataDxfId="139">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table610" displayName="Table610" ref="W3:W8" totalsRowShown="0" headerRowDxfId="120" dataDxfId="119">
   <autoFilter ref="W3:W8"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Timezone" dataDxfId="138"/>
+    <tableColumn id="1" name="Timezone" dataDxfId="118"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table61013" displayName="Table61013" ref="Y3:Y6" totalsRowShown="0" headerRowDxfId="137" dataDxfId="136">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table61013" displayName="Table61013" ref="Y3:Y6" totalsRowShown="0" headerRowDxfId="117" dataDxfId="116">
   <autoFilter ref="Y3:Y6"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="SNMP Version" dataDxfId="135"/>
+    <tableColumn id="1" name="SNMP Version" dataDxfId="115"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table15" displayName="Table15" ref="AA3:AA5" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table15" displayName="Table15" ref="AA3:AA5" totalsRowShown="0" headerRowDxfId="114" dataDxfId="113">
   <autoFilter ref="AA3:AA5"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="SNMP Permission" dataDxfId="132"/>
+    <tableColumn id="1" name="SNMP Permission" dataDxfId="112"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table16" displayName="Table16" ref="AC3:AC27" totalsRowShown="0" headerRowDxfId="131" dataDxfId="130">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table16" displayName="Table16" ref="AC3:AC27" totalsRowShown="0" headerRowDxfId="111" dataDxfId="110">
   <autoFilter ref="AC3:AC27"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Syslog Facility" dataDxfId="129"/>
+    <tableColumn id="1" name="Syslog Facility" dataDxfId="109"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12881,7 +12880,7 @@
   </sheetPr>
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -13594,7 +13593,7 @@
   </sheetPr>
   <dimension ref="A1:Y89"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
@@ -16174,12 +16173,12 @@
     <mergeCell ref="V10:X10"/>
   </mergeCells>
   <conditionalFormatting sqref="F53:F54">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="2" stopIfTrue="1">
       <formula>E53=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F59">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="1" stopIfTrue="1">
       <formula>E59=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17016,37 +17015,37 @@
     <mergeCell ref="B9:D9"/>
   </mergeCells>
   <conditionalFormatting sqref="B4 E4">
-    <cfRule type="expression" dxfId="29" priority="7">
+    <cfRule type="expression" dxfId="162" priority="7">
       <formula>B4=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:H9">
-    <cfRule type="expression" dxfId="28" priority="6">
+    <cfRule type="expression" dxfId="161" priority="6">
       <formula>B$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:H16">
-    <cfRule type="expression" dxfId="27" priority="5">
+    <cfRule type="expression" dxfId="160" priority="5">
       <formula>C13=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:H23">
-    <cfRule type="expression" dxfId="26" priority="4">
+    <cfRule type="expression" dxfId="159" priority="4">
       <formula>C20=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:H28">
-    <cfRule type="expression" dxfId="25" priority="3">
+    <cfRule type="expression" dxfId="158" priority="3">
       <formula>C25=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:E34">
-    <cfRule type="expression" dxfId="24" priority="2">
+    <cfRule type="expression" dxfId="157" priority="2">
       <formula>C31=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F31:H34">
-    <cfRule type="expression" dxfId="23" priority="1">
+    <cfRule type="expression" dxfId="156" priority="1">
       <formula>F31=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17612,7 +17611,7 @@
   <dimension ref="S3:W15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -17849,7 +17848,7 @@
   </sheetPr>
   <dimension ref="A1:AC76"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -18964,67 +18963,67 @@
     <mergeCell ref="B37:C37"/>
   </mergeCells>
   <conditionalFormatting sqref="C11:C25">
-    <cfRule type="expression" dxfId="22" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="9" stopIfTrue="1">
       <formula>$C11=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C8">
-    <cfRule type="expression" dxfId="21" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="8" stopIfTrue="1">
       <formula>$C5=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:C35">
-    <cfRule type="expression" dxfId="20" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="137" priority="11" stopIfTrue="1">
       <formula>$C32=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C29">
-    <cfRule type="expression" dxfId="19" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="136" priority="10" stopIfTrue="1">
       <formula>$C28=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C41">
-    <cfRule type="expression" dxfId="18" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="135" priority="12" stopIfTrue="1">
       <formula>$C38=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47:C48">
-    <cfRule type="expression" dxfId="17" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="134" priority="3" stopIfTrue="1">
       <formula>$C$46=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50:C51">
-    <cfRule type="expression" dxfId="16" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="133" priority="4" stopIfTrue="1">
       <formula>$C$49=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53:C54">
-    <cfRule type="expression" dxfId="15" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="5" stopIfTrue="1">
       <formula>$C$52=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44:C72">
-    <cfRule type="expression" dxfId="14" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="13" stopIfTrue="1">
       <formula>$C44=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B56:C59">
-    <cfRule type="expression" dxfId="13" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="130" priority="6" stopIfTrue="1">
       <formula>$C$55=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B61:C64">
-    <cfRule type="expression" dxfId="12" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="7" stopIfTrue="1">
       <formula>$C$60=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B66:C68">
-    <cfRule type="expression" dxfId="11" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="2" stopIfTrue="1">
       <formula>$C$65=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B70:C72">
-    <cfRule type="expression" dxfId="10" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="1" stopIfTrue="1">
       <formula>$C$69=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19092,9 +19091,9 @@
   </sheetPr>
   <dimension ref="A1:U45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20770,7 +20769,7 @@
   </sheetPr>
   <dimension ref="A2:X57"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="T6" sqref="T6:W6"/>
     </sheetView>
@@ -23086,32 +23085,32 @@
     <mergeCell ref="R14:W14"/>
   </mergeCells>
   <conditionalFormatting sqref="F37:F43 F46:F48">
-    <cfRule type="expression" dxfId="9" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="6" stopIfTrue="1">
       <formula>E37=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21:F34">
-    <cfRule type="expression" dxfId="8" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="5" stopIfTrue="1">
       <formula>E20=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F11 F16:F18">
-    <cfRule type="expression" dxfId="7" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="4" stopIfTrue="1">
       <formula>E5=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57">
-    <cfRule type="expression" dxfId="6" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="3" stopIfTrue="1">
       <formula>E57=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52">
-    <cfRule type="expression" dxfId="5" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="2" stopIfTrue="1">
       <formula>E52=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44:F45">
-    <cfRule type="expression" dxfId="4" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="1" stopIfTrue="1">
       <formula>E43=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23142,9 +23141,9 @@
   </sheetPr>
   <dimension ref="A1:Z58"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="P50" sqref="P50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -25447,12 +25446,12 @@
     <mergeCell ref="T19:Y19"/>
   </mergeCells>
   <conditionalFormatting sqref="F52:F53">
-    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="2" stopIfTrue="1">
       <formula>E52=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F58">
-    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="1" stopIfTrue="1">
       <formula>E58=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25474,6 +25473,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001185193EED7D7C45B2181268987EEB31" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0398fff93780d69aa75df20e85be37f6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="55e0dd24fae28f1b5dd5f79afbe3cfeb">
     <xsd:element name="properties">
@@ -25587,22 +25601,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7243C670-E16E-4DBD-9932-9E3C368D5054}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42535616-3E13-4575-9B51-ECA7D821FF84}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5245AC5-DF56-430A-AECE-726FB05E2AD0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25616,27 +25638,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7243C670-E16E-4DBD-9932-9E3C368D5054}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42535616-3E13-4575-9B51-ECA7D821FF84}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modified network diagram to match RA
</commit_message>
<xml_diff>
--- a/data/sample_switch_configs/Solution-Workbook.xlsx
+++ b/data/sample_switch_configs/Solution-Workbook.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6760" tabRatio="782"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6760" tabRatio="782" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -6254,45 +6254,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="39" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="40" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="41" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="37" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="6" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="38" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="28" borderId="19" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="20" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="21" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="34" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="35" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="26" borderId="35" xfId="141" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="36" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="37" fillId="26" borderId="19" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -6332,45 +6293,48 @@
     <xf numFmtId="0" fontId="43" fillId="27" borderId="33" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="27" borderId="58" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="27" borderId="12" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="27" borderId="59" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="41" borderId="58" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="41" borderId="12" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="41" borderId="59" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="27" borderId="31" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="27" borderId="32" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="27" borderId="33" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="44" fillId="28" borderId="19" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="20" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="21" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="34" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="35" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="26" borderId="35" xfId="141" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="36" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="39" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="40" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="41" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="37" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="6" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="38" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="41" borderId="39" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="60" fillId="41" borderId="40" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="53" fillId="41" borderId="40" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -6383,94 +6347,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="19" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="20" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="21" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="22" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="23" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="24" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="8" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="25" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="81" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="81" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="81" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="27" borderId="82" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="27" borderId="77" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="27" borderId="83" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="58" xfId="112" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="12" xfId="112" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="59" xfId="112" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="41" borderId="39" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="60" fillId="41" borderId="40" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="53" fillId="41" borderId="40" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -6484,6 +6360,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="88" fillId="0" borderId="58" xfId="1629" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="58" xfId="112" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -6501,6 +6381,126 @@
     <xf numFmtId="0" fontId="60" fillId="41" borderId="37" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="60" fillId="41" borderId="6" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="53" fillId="41" borderId="6" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="41" borderId="58" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="41" borderId="12" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="41" borderId="59" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="12" xfId="112" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="59" xfId="112" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="82" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="12" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="59" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="77" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="83" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="58" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="27" borderId="31" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="27" borderId="32" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="27" borderId="33" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="19" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="20" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="21" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="22" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="23" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="24" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="8" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="25" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="81" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="81" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="81" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="48" fillId="25" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6527,63 +6527,90 @@
     <xf numFmtId="0" fontId="49" fillId="25" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="37" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="36" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="31" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="31" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="33" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="31" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="31" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="31" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="31" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="31" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="31" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="36" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="36" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="36" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="32" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="38" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="32" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="57" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="57" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="46" fillId="31" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="31" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="32" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="33" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="38" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="32" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="37" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="36" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="46" fillId="31" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="31" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="31" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="31" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="31" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="31" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="36" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="36" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="36" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="32" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="32" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="32" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="38" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="38" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="38" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -6596,32 +6623,14 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="38" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="36" fillId="38" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="36" fillId="38" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="36" fillId="32" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="32" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="32" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="36" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="36" fillId="36" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -6630,15 +6639,6 @@
     </xf>
     <xf numFmtId="0" fontId="36" fillId="33" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="38" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -10239,14 +10239,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>196850</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>36510</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>94588</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -10267,7 +10267,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8121650" cy="6697660"/>
+          <a:ext cx="10579100" cy="8724238"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12880,7 +12880,7 @@
   </sheetPr>
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -12980,19 +12980,19 @@
     </row>
     <row r="7" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
-      <c r="B7" s="208" t="s">
+      <c r="B7" s="195" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="209"/>
-      <c r="D7" s="209"/>
-      <c r="E7" s="209"/>
-      <c r="F7" s="209"/>
-      <c r="G7" s="209"/>
-      <c r="H7" s="209"/>
-      <c r="I7" s="209"/>
-      <c r="J7" s="209"/>
-      <c r="K7" s="209"/>
-      <c r="L7" s="210"/>
+      <c r="C7" s="196"/>
+      <c r="D7" s="196"/>
+      <c r="E7" s="196"/>
+      <c r="F7" s="196"/>
+      <c r="G7" s="196"/>
+      <c r="H7" s="196"/>
+      <c r="I7" s="196"/>
+      <c r="J7" s="196"/>
+      <c r="K7" s="196"/>
+      <c r="L7" s="197"/>
       <c r="M7" s="9"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -13080,19 +13080,19 @@
     </row>
     <row r="13" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
-      <c r="B13" s="211" t="s">
+      <c r="B13" s="198" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="212"/>
-      <c r="D13" s="212"/>
-      <c r="E13" s="212"/>
-      <c r="F13" s="212"/>
-      <c r="G13" s="212"/>
-      <c r="H13" s="212"/>
-      <c r="I13" s="212"/>
-      <c r="J13" s="212"/>
-      <c r="K13" s="212"/>
-      <c r="L13" s="213"/>
+      <c r="C13" s="199"/>
+      <c r="D13" s="199"/>
+      <c r="E13" s="199"/>
+      <c r="F13" s="199"/>
+      <c r="G13" s="199"/>
+      <c r="H13" s="199"/>
+      <c r="I13" s="199"/>
+      <c r="J13" s="199"/>
+      <c r="K13" s="199"/>
+      <c r="L13" s="200"/>
       <c r="M13" s="9"/>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -13180,19 +13180,19 @@
     </row>
     <row r="19" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
-      <c r="B19" s="214" t="s">
+      <c r="B19" s="201" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="215"/>
-      <c r="D19" s="215"/>
-      <c r="E19" s="215"/>
-      <c r="F19" s="215"/>
-      <c r="G19" s="215"/>
-      <c r="H19" s="215"/>
-      <c r="I19" s="215"/>
-      <c r="J19" s="215"/>
-      <c r="K19" s="215"/>
-      <c r="L19" s="216"/>
+      <c r="C19" s="202"/>
+      <c r="D19" s="202"/>
+      <c r="E19" s="202"/>
+      <c r="F19" s="202"/>
+      <c r="G19" s="202"/>
+      <c r="H19" s="202"/>
+      <c r="I19" s="202"/>
+      <c r="J19" s="202"/>
+      <c r="K19" s="202"/>
+      <c r="L19" s="203"/>
       <c r="M19" s="9"/>
     </row>
     <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -13263,19 +13263,19 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
-      <c r="B24" s="217" t="s">
+      <c r="B24" s="204" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="218"/>
-      <c r="D24" s="218"/>
-      <c r="E24" s="218"/>
-      <c r="F24" s="218"/>
-      <c r="G24" s="218"/>
-      <c r="H24" s="218"/>
-      <c r="I24" s="218"/>
-      <c r="J24" s="218"/>
-      <c r="K24" s="218"/>
-      <c r="L24" s="219"/>
+      <c r="C24" s="205"/>
+      <c r="D24" s="205"/>
+      <c r="E24" s="205"/>
+      <c r="F24" s="205"/>
+      <c r="G24" s="205"/>
+      <c r="H24" s="205"/>
+      <c r="I24" s="205"/>
+      <c r="J24" s="205"/>
+      <c r="K24" s="205"/>
+      <c r="L24" s="206"/>
       <c r="M24" s="9"/>
     </row>
     <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -13431,110 +13431,110 @@
     </row>
     <row r="34" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="4"/>
-      <c r="B34" s="220" t="s">
+      <c r="B34" s="207" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="221"/>
-      <c r="D34" s="221"/>
-      <c r="E34" s="221"/>
-      <c r="F34" s="221"/>
-      <c r="G34" s="221"/>
-      <c r="H34" s="221"/>
-      <c r="I34" s="221"/>
-      <c r="J34" s="221"/>
-      <c r="K34" s="221"/>
-      <c r="L34" s="222"/>
+      <c r="C34" s="208"/>
+      <c r="D34" s="208"/>
+      <c r="E34" s="208"/>
+      <c r="F34" s="208"/>
+      <c r="G34" s="208"/>
+      <c r="H34" s="208"/>
+      <c r="I34" s="208"/>
+      <c r="J34" s="208"/>
+      <c r="K34" s="208"/>
+      <c r="L34" s="209"/>
       <c r="M34" s="9"/>
     </row>
     <row r="35" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="4"/>
-      <c r="B35" s="201" t="s">
+      <c r="B35" s="210" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="202"/>
-      <c r="D35" s="203"/>
-      <c r="E35" s="201" t="s">
+      <c r="C35" s="211"/>
+      <c r="D35" s="212"/>
+      <c r="E35" s="210" t="s">
         <v>26</v>
       </c>
-      <c r="F35" s="202"/>
-      <c r="G35" s="203"/>
-      <c r="H35" s="201" t="s">
+      <c r="F35" s="211"/>
+      <c r="G35" s="212"/>
+      <c r="H35" s="210" t="s">
         <v>27</v>
       </c>
-      <c r="I35" s="202"/>
-      <c r="J35" s="203"/>
-      <c r="K35" s="201" t="s">
+      <c r="I35" s="211"/>
+      <c r="J35" s="212"/>
+      <c r="K35" s="210" t="s">
         <v>28</v>
       </c>
-      <c r="L35" s="203"/>
+      <c r="L35" s="212"/>
       <c r="M35" s="9"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="4"/>
-      <c r="B36" s="204">
+      <c r="B36" s="213">
         <v>1</v>
       </c>
-      <c r="C36" s="205"/>
-      <c r="D36" s="205"/>
-      <c r="E36" s="206"/>
-      <c r="F36" s="205"/>
-      <c r="G36" s="205"/>
-      <c r="H36" s="205"/>
-      <c r="I36" s="205"/>
-      <c r="J36" s="205"/>
-      <c r="K36" s="205"/>
-      <c r="L36" s="207"/>
+      <c r="C36" s="214"/>
+      <c r="D36" s="214"/>
+      <c r="E36" s="215"/>
+      <c r="F36" s="214"/>
+      <c r="G36" s="214"/>
+      <c r="H36" s="214"/>
+      <c r="I36" s="214"/>
+      <c r="J36" s="214"/>
+      <c r="K36" s="214"/>
+      <c r="L36" s="216"/>
       <c r="M36" s="9"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="4"/>
-      <c r="B37" s="198">
+      <c r="B37" s="220">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C37" s="199"/>
-      <c r="D37" s="199"/>
-      <c r="E37" s="199"/>
-      <c r="F37" s="199"/>
-      <c r="G37" s="199"/>
-      <c r="H37" s="199"/>
-      <c r="I37" s="199"/>
-      <c r="J37" s="199"/>
-      <c r="K37" s="199"/>
-      <c r="L37" s="200"/>
+      <c r="C37" s="221"/>
+      <c r="D37" s="221"/>
+      <c r="E37" s="221"/>
+      <c r="F37" s="221"/>
+      <c r="G37" s="221"/>
+      <c r="H37" s="221"/>
+      <c r="I37" s="221"/>
+      <c r="J37" s="221"/>
+      <c r="K37" s="221"/>
+      <c r="L37" s="222"/>
       <c r="M37" s="9"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="4"/>
-      <c r="B38" s="198">
+      <c r="B38" s="220">
         <v>1.2</v>
       </c>
-      <c r="C38" s="199"/>
-      <c r="D38" s="199"/>
-      <c r="E38" s="199"/>
-      <c r="F38" s="199"/>
-      <c r="G38" s="199"/>
-      <c r="H38" s="199"/>
-      <c r="I38" s="199"/>
-      <c r="J38" s="199"/>
-      <c r="K38" s="199"/>
-      <c r="L38" s="200"/>
+      <c r="C38" s="221"/>
+      <c r="D38" s="221"/>
+      <c r="E38" s="221"/>
+      <c r="F38" s="221"/>
+      <c r="G38" s="221"/>
+      <c r="H38" s="221"/>
+      <c r="I38" s="221"/>
+      <c r="J38" s="221"/>
+      <c r="K38" s="221"/>
+      <c r="L38" s="222"/>
       <c r="M38" s="9"/>
     </row>
     <row r="39" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="4"/>
-      <c r="B39" s="195">
+      <c r="B39" s="217">
         <v>1.3</v>
       </c>
-      <c r="C39" s="196"/>
-      <c r="D39" s="196"/>
-      <c r="E39" s="196"/>
-      <c r="F39" s="196"/>
-      <c r="G39" s="196"/>
-      <c r="H39" s="196"/>
-      <c r="I39" s="196"/>
-      <c r="J39" s="196"/>
-      <c r="K39" s="196"/>
-      <c r="L39" s="197"/>
+      <c r="C39" s="218"/>
+      <c r="D39" s="218"/>
+      <c r="E39" s="218"/>
+      <c r="F39" s="218"/>
+      <c r="G39" s="218"/>
+      <c r="H39" s="218"/>
+      <c r="I39" s="218"/>
+      <c r="J39" s="218"/>
+      <c r="K39" s="218"/>
+      <c r="L39" s="219"/>
       <c r="M39" s="9"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.35">
@@ -13554,19 +13554,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B7:L7"/>
-    <mergeCell ref="B13:L13"/>
-    <mergeCell ref="B19:L19"/>
-    <mergeCell ref="B24:L24"/>
-    <mergeCell ref="B34:L34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:J35"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="K36:L36"/>
     <mergeCell ref="B39:D39"/>
     <mergeCell ref="E39:G39"/>
     <mergeCell ref="H39:J39"/>
@@ -13579,6 +13566,19 @@
     <mergeCell ref="E38:G38"/>
     <mergeCell ref="H38:J38"/>
     <mergeCell ref="K38:L38"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:J35"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="B7:L7"/>
+    <mergeCell ref="B13:L13"/>
+    <mergeCell ref="B19:L19"/>
+    <mergeCell ref="B24:L24"/>
+    <mergeCell ref="B34:L34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -13629,21 +13629,21 @@
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
-      <c r="E2" s="286" t="s">
+      <c r="E2" s="300" t="s">
         <v>308</v>
       </c>
-      <c r="F2" s="286"/>
-      <c r="G2" s="286"/>
-      <c r="H2" s="286"/>
-      <c r="I2" s="286"/>
-      <c r="J2" s="286"/>
-      <c r="K2" s="286"/>
-      <c r="L2" s="286"/>
-      <c r="M2" s="286"/>
-      <c r="N2" s="286"/>
-      <c r="O2" s="286"/>
-      <c r="P2" s="286"/>
-      <c r="Q2" s="286"/>
+      <c r="F2" s="300"/>
+      <c r="G2" s="300"/>
+      <c r="H2" s="300"/>
+      <c r="I2" s="300"/>
+      <c r="J2" s="300"/>
+      <c r="K2" s="300"/>
+      <c r="L2" s="300"/>
+      <c r="M2" s="300"/>
+      <c r="N2" s="300"/>
+      <c r="O2" s="300"/>
+      <c r="P2" s="300"/>
+      <c r="Q2" s="300"/>
       <c r="S2" s="125"/>
       <c r="T2" s="125"/>
       <c r="U2" s="125"/>
@@ -13653,44 +13653,44 @@
       <c r="Y2" s="125"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A3" s="292" t="s">
+      <c r="A3" s="291" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="293"/>
+      <c r="B3" s="292"/>
       <c r="C3" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="E3" s="294" t="s">
+      <c r="E3" s="304" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="289"/>
-      <c r="G3" s="289" t="s">
+      <c r="F3" s="302"/>
+      <c r="G3" s="302" t="s">
         <v>49</v>
       </c>
-      <c r="H3" s="289"/>
-      <c r="I3" s="289" t="s">
+      <c r="H3" s="302"/>
+      <c r="I3" s="302" t="s">
         <v>44</v>
       </c>
-      <c r="J3" s="289"/>
+      <c r="J3" s="302"/>
       <c r="K3" s="151"/>
-      <c r="L3" s="295" t="s">
+      <c r="L3" s="305" t="s">
         <v>298</v>
       </c>
-      <c r="M3" s="296"/>
-      <c r="N3" s="296"/>
-      <c r="O3" s="297"/>
-      <c r="P3" s="289" t="s">
+      <c r="M3" s="306"/>
+      <c r="N3" s="306"/>
+      <c r="O3" s="307"/>
+      <c r="P3" s="302" t="s">
         <v>45</v>
       </c>
-      <c r="Q3" s="290"/>
-      <c r="S3" s="324" t="s">
+      <c r="Q3" s="303"/>
+      <c r="S3" s="327" t="s">
         <v>54</v>
       </c>
-      <c r="T3" s="325"/>
-      <c r="U3" s="320"/>
-      <c r="V3" s="321"/>
-      <c r="W3" s="321"/>
-      <c r="X3" s="322"/>
+      <c r="T3" s="328"/>
+      <c r="U3" s="315"/>
+      <c r="V3" s="316"/>
+      <c r="W3" s="316"/>
+      <c r="X3" s="317"/>
       <c r="Y3" s="146"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.35">
@@ -13742,14 +13742,14 @@
       <c r="Q4" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="S4" s="326" t="s">
+      <c r="S4" s="329" t="s">
         <v>53</v>
       </c>
-      <c r="T4" s="327"/>
-      <c r="U4" s="320"/>
-      <c r="V4" s="321"/>
-      <c r="W4" s="321"/>
-      <c r="X4" s="322"/>
+      <c r="T4" s="330"/>
+      <c r="U4" s="315"/>
+      <c r="V4" s="316"/>
+      <c r="W4" s="316"/>
+      <c r="X4" s="317"/>
       <c r="Y4" s="146"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.35">
@@ -13804,14 +13804,14 @@
       <c r="Q5" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="S5" s="324" t="s">
+      <c r="S5" s="327" t="s">
         <v>42</v>
       </c>
-      <c r="T5" s="325"/>
-      <c r="U5" s="320"/>
-      <c r="V5" s="321"/>
-      <c r="W5" s="321"/>
-      <c r="X5" s="322"/>
+      <c r="T5" s="328"/>
+      <c r="U5" s="315"/>
+      <c r="V5" s="316"/>
+      <c r="W5" s="316"/>
+      <c r="X5" s="317"/>
       <c r="Y5" s="146"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.35">
@@ -13866,17 +13866,17 @@
       <c r="Q6" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="S6" s="326" t="s">
+      <c r="S6" s="329" t="s">
         <v>71</v>
       </c>
-      <c r="T6" s="327"/>
-      <c r="U6" s="320" t="str">
+      <c r="T6" s="330"/>
+      <c r="U6" s="315" t="str">
         <f>S4048_2_FW</f>
         <v>fw: 9.11(0.0P2)</v>
       </c>
-      <c r="V6" s="321"/>
-      <c r="W6" s="321"/>
-      <c r="X6" s="322"/>
+      <c r="V6" s="316"/>
+      <c r="W6" s="316"/>
+      <c r="X6" s="317"/>
       <c r="Y6" s="146"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.35">
@@ -13984,16 +13984,16 @@
       <c r="Q8" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="S8" s="317" t="s">
+      <c r="S8" s="312" t="s">
         <v>167</v>
       </c>
-      <c r="T8" s="318"/>
-      <c r="U8" s="319"/>
-      <c r="V8" s="328" t="s">
+      <c r="T8" s="313"/>
+      <c r="U8" s="314"/>
+      <c r="V8" s="324" t="s">
         <v>289</v>
       </c>
-      <c r="W8" s="329"/>
-      <c r="X8" s="330"/>
+      <c r="W8" s="325"/>
+      <c r="X8" s="326"/>
       <c r="Y8" s="139"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.35">
@@ -14053,9 +14053,9 @@
       </c>
       <c r="T9" s="332"/>
       <c r="U9" s="333"/>
-      <c r="V9" s="320"/>
-      <c r="W9" s="321"/>
-      <c r="X9" s="322"/>
+      <c r="V9" s="315"/>
+      <c r="W9" s="316"/>
+      <c r="X9" s="317"/>
       <c r="Y9" s="146"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.35">
@@ -14115,11 +14115,11 @@
       </c>
       <c r="T10" s="335"/>
       <c r="U10" s="336"/>
-      <c r="V10" s="320">
+      <c r="V10" s="315">
         <v>20480</v>
       </c>
-      <c r="W10" s="321"/>
-      <c r="X10" s="322"/>
+      <c r="W10" s="316"/>
+      <c r="X10" s="317"/>
       <c r="Y10" s="146"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.35">
@@ -14210,14 +14210,14 @@
       <c r="O12" s="130"/>
       <c r="P12" s="48"/>
       <c r="Q12" s="61"/>
-      <c r="S12" s="317" t="s">
+      <c r="S12" s="312" t="s">
         <v>59</v>
       </c>
-      <c r="T12" s="318"/>
-      <c r="U12" s="319"/>
-      <c r="V12" s="320"/>
-      <c r="W12" s="321"/>
-      <c r="X12" s="322"/>
+      <c r="T12" s="313"/>
+      <c r="U12" s="314"/>
+      <c r="V12" s="315"/>
+      <c r="W12" s="316"/>
+      <c r="X12" s="317"/>
       <c r="Y12" s="146"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.35">
@@ -14254,24 +14254,24 @@
       <c r="O13" s="130"/>
       <c r="P13" s="48"/>
       <c r="Q13" s="61"/>
-      <c r="S13" s="314" t="s">
+      <c r="S13" s="318" t="s">
         <v>60</v>
       </c>
-      <c r="T13" s="315"/>
-      <c r="U13" s="316"/>
-      <c r="V13" s="328">
+      <c r="T13" s="319"/>
+      <c r="U13" s="320"/>
+      <c r="V13" s="324">
         <f>VLTDOMAIN</f>
         <v>1</v>
       </c>
-      <c r="W13" s="329"/>
-      <c r="X13" s="330"/>
+      <c r="W13" s="325"/>
+      <c r="X13" s="326"/>
       <c r="Y13" s="139"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A14" s="294" t="s">
+      <c r="A14" s="304" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="290"/>
+      <c r="B14" s="303"/>
       <c r="E14" s="36" t="s">
         <v>239</v>
       </c>
@@ -14295,16 +14295,16 @@
       <c r="O14" s="130"/>
       <c r="P14" s="48"/>
       <c r="Q14" s="61"/>
-      <c r="S14" s="314" t="s">
+      <c r="S14" s="318" t="s">
         <v>166</v>
       </c>
-      <c r="T14" s="315"/>
-      <c r="U14" s="316"/>
-      <c r="V14" s="320">
+      <c r="T14" s="319"/>
+      <c r="U14" s="320"/>
+      <c r="V14" s="315">
         <v>2</v>
       </c>
-      <c r="W14" s="321"/>
-      <c r="X14" s="322"/>
+      <c r="W14" s="316"/>
+      <c r="X14" s="317"/>
       <c r="Y14" s="146"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.35">
@@ -14337,16 +14337,16 @@
       <c r="O15" s="130"/>
       <c r="P15" s="48"/>
       <c r="Q15" s="61"/>
-      <c r="S15" s="317" t="s">
+      <c r="S15" s="312" t="s">
         <v>67</v>
       </c>
-      <c r="T15" s="318"/>
-      <c r="U15" s="319"/>
-      <c r="V15" s="320">
+      <c r="T15" s="313"/>
+      <c r="U15" s="314"/>
+      <c r="V15" s="315">
         <v>1</v>
       </c>
-      <c r="W15" s="321"/>
-      <c r="X15" s="322"/>
+      <c r="W15" s="316"/>
+      <c r="X15" s="317"/>
       <c r="Y15" s="146"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.35">
@@ -14444,14 +14444,14 @@
       <c r="Q17" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="S17" s="298" t="s">
+      <c r="S17" s="308" t="s">
         <v>70</v>
       </c>
-      <c r="T17" s="299"/>
-      <c r="U17" s="299"/>
-      <c r="V17" s="299"/>
-      <c r="W17" s="299"/>
-      <c r="X17" s="300"/>
+      <c r="T17" s="309"/>
+      <c r="U17" s="309"/>
+      <c r="V17" s="309"/>
+      <c r="W17" s="309"/>
+      <c r="X17" s="310"/>
       <c r="Y17" s="140"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.35">
@@ -14500,12 +14500,12 @@
       <c r="Q18" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="S18" s="305"/>
-      <c r="T18" s="306"/>
-      <c r="U18" s="306"/>
-      <c r="V18" s="306"/>
-      <c r="W18" s="306"/>
-      <c r="X18" s="307"/>
+      <c r="S18" s="285"/>
+      <c r="T18" s="286"/>
+      <c r="U18" s="286"/>
+      <c r="V18" s="286"/>
+      <c r="W18" s="286"/>
+      <c r="X18" s="287"/>
       <c r="Y18" s="141"/>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.35">
@@ -14539,12 +14539,12 @@
       <c r="Q19" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="S19" s="308"/>
-      <c r="T19" s="309"/>
-      <c r="U19" s="309"/>
-      <c r="V19" s="309"/>
-      <c r="W19" s="309"/>
-      <c r="X19" s="310"/>
+      <c r="S19" s="288"/>
+      <c r="T19" s="289"/>
+      <c r="U19" s="289"/>
+      <c r="V19" s="289"/>
+      <c r="W19" s="289"/>
+      <c r="X19" s="290"/>
       <c r="Y19" s="141"/>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.35">
@@ -14578,12 +14578,12 @@
       <c r="Q20" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="S20" s="305"/>
-      <c r="T20" s="306"/>
-      <c r="U20" s="306"/>
-      <c r="V20" s="306"/>
-      <c r="W20" s="306"/>
-      <c r="X20" s="307"/>
+      <c r="S20" s="285"/>
+      <c r="T20" s="286"/>
+      <c r="U20" s="286"/>
+      <c r="V20" s="286"/>
+      <c r="W20" s="286"/>
+      <c r="X20" s="287"/>
       <c r="Y20" s="141"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.35">
@@ -14613,12 +14613,12 @@
       <c r="Q21" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="S21" s="308"/>
-      <c r="T21" s="309"/>
-      <c r="U21" s="309"/>
-      <c r="V21" s="309"/>
-      <c r="W21" s="309"/>
-      <c r="X21" s="310"/>
+      <c r="S21" s="288"/>
+      <c r="T21" s="289"/>
+      <c r="U21" s="289"/>
+      <c r="V21" s="289"/>
+      <c r="W21" s="289"/>
+      <c r="X21" s="290"/>
       <c r="Y21" s="141"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.35">
@@ -14964,9 +14964,9 @@
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A32" s="285"/>
-      <c r="B32" s="285"/>
-      <c r="C32" s="285"/>
+      <c r="A32" s="299"/>
+      <c r="B32" s="299"/>
+      <c r="C32" s="299"/>
       <c r="E32" s="36" t="s">
         <v>257</v>
       </c>
@@ -15009,9 +15009,9 @@
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A33" s="285"/>
-      <c r="B33" s="285"/>
-      <c r="C33" s="285"/>
+      <c r="A33" s="299"/>
+      <c r="B33" s="299"/>
+      <c r="C33" s="299"/>
       <c r="E33" s="36" t="s">
         <v>258</v>
       </c>
@@ -15054,9 +15054,9 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A34" s="285"/>
-      <c r="B34" s="285"/>
-      <c r="C34" s="285"/>
+      <c r="A34" s="299"/>
+      <c r="B34" s="299"/>
+      <c r="C34" s="299"/>
       <c r="E34" s="36" t="s">
         <v>259</v>
       </c>
@@ -15141,10 +15141,10 @@
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A36" s="323" t="s">
+      <c r="A36" s="311" t="s">
         <v>402</v>
       </c>
-      <c r="B36" s="323"/>
+      <c r="B36" s="311"/>
       <c r="E36" s="36" t="s">
         <v>261</v>
       </c>
@@ -15170,8 +15170,8 @@
       <c r="Q36" s="61"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A37" s="323"/>
-      <c r="B37" s="323"/>
+      <c r="A37" s="311"/>
+      <c r="B37" s="311"/>
       <c r="E37" s="36" t="s">
         <v>262</v>
       </c>
@@ -15197,10 +15197,10 @@
       <c r="Q37" s="61"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A38" s="292" t="s">
+      <c r="A38" s="291" t="s">
         <v>65</v>
       </c>
-      <c r="B38" s="293"/>
+      <c r="B38" s="292"/>
       <c r="E38" s="36" t="s">
         <v>263</v>
       </c>
@@ -16133,6 +16133,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="A32:C34"/>
+    <mergeCell ref="S20:X20"/>
+    <mergeCell ref="S21:X21"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:X3"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:X4"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:X5"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="U6:X6"/>
+    <mergeCell ref="V8:X8"/>
+    <mergeCell ref="S9:U9"/>
+    <mergeCell ref="V9:X9"/>
+    <mergeCell ref="S10:U10"/>
+    <mergeCell ref="V10:X10"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="E2:Q2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="P3:Q3"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="L3:O3"/>
     <mergeCell ref="A3:B3"/>
@@ -16149,28 +16171,6 @@
     <mergeCell ref="S15:U15"/>
     <mergeCell ref="V15:X15"/>
     <mergeCell ref="S17:X17"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="E2:Q2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="A32:C34"/>
-    <mergeCell ref="S20:X20"/>
-    <mergeCell ref="S21:X21"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:X3"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:X4"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:X5"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="U6:X6"/>
-    <mergeCell ref="V8:X8"/>
-    <mergeCell ref="S9:U9"/>
-    <mergeCell ref="V9:X9"/>
-    <mergeCell ref="S10:U10"/>
-    <mergeCell ref="V10:X10"/>
   </mergeCells>
   <conditionalFormatting sqref="F53:F54">
     <cfRule type="expression" dxfId="26" priority="2" stopIfTrue="1">
@@ -16243,15 +16243,15 @@
     </row>
     <row r="2" spans="1:14" s="73" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="72"/>
-      <c r="B2" s="223" t="s">
+      <c r="B2" s="256" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="224"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="224"/>
-      <c r="F2" s="224"/>
-      <c r="G2" s="224"/>
-      <c r="H2" s="225"/>
+      <c r="C2" s="252"/>
+      <c r="D2" s="252"/>
+      <c r="E2" s="252"/>
+      <c r="F2" s="252"/>
+      <c r="G2" s="252"/>
+      <c r="H2" s="253"/>
       <c r="I2" s="72"/>
       <c r="J2" s="72"/>
       <c r="K2" s="72"/>
@@ -16261,124 +16261,124 @@
     </row>
     <row r="3" spans="1:14" s="73" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="72"/>
-      <c r="B3" s="226" t="s">
+      <c r="B3" s="245" t="s">
         <v>140</v>
       </c>
-      <c r="C3" s="227"/>
-      <c r="D3" s="228"/>
-      <c r="E3" s="226" t="s">
+      <c r="C3" s="246"/>
+      <c r="D3" s="247"/>
+      <c r="E3" s="245" t="s">
         <v>141</v>
       </c>
-      <c r="F3" s="227"/>
-      <c r="G3" s="227"/>
-      <c r="H3" s="228"/>
+      <c r="F3" s="246"/>
+      <c r="G3" s="246"/>
+      <c r="H3" s="247"/>
       <c r="I3" s="72"/>
       <c r="J3" s="72"/>
-      <c r="K3" s="229" t="s">
+      <c r="K3" s="257" t="s">
         <v>142</v>
       </c>
-      <c r="L3" s="230"/>
-      <c r="M3" s="231"/>
+      <c r="L3" s="258"/>
+      <c r="M3" s="259"/>
       <c r="N3" s="72"/>
     </row>
     <row r="4" spans="1:14" s="73" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="72"/>
-      <c r="B4" s="232"/>
-      <c r="C4" s="233"/>
-      <c r="D4" s="234"/>
-      <c r="E4" s="235"/>
-      <c r="F4" s="236"/>
-      <c r="G4" s="236"/>
-      <c r="H4" s="237"/>
+      <c r="B4" s="242"/>
+      <c r="C4" s="243"/>
+      <c r="D4" s="244"/>
+      <c r="E4" s="226"/>
+      <c r="F4" s="227"/>
+      <c r="G4" s="227"/>
+      <c r="H4" s="228"/>
       <c r="I4" s="72"/>
       <c r="J4" s="72"/>
-      <c r="K4" s="238"/>
-      <c r="L4" s="239"/>
-      <c r="M4" s="240"/>
+      <c r="K4" s="260"/>
+      <c r="L4" s="261"/>
+      <c r="M4" s="262"/>
       <c r="N4" s="72"/>
     </row>
     <row r="5" spans="1:14" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="72"/>
-      <c r="B5" s="226" t="s">
+      <c r="B5" s="245" t="s">
         <v>200</v>
       </c>
-      <c r="C5" s="227"/>
-      <c r="D5" s="227"/>
-      <c r="E5" s="226" t="s">
+      <c r="C5" s="246"/>
+      <c r="D5" s="246"/>
+      <c r="E5" s="245" t="s">
         <v>143</v>
       </c>
-      <c r="F5" s="227"/>
-      <c r="G5" s="227"/>
-      <c r="H5" s="228"/>
+      <c r="F5" s="246"/>
+      <c r="G5" s="246"/>
+      <c r="H5" s="247"/>
       <c r="I5" s="72"/>
       <c r="J5" s="74"/>
-      <c r="K5" s="241"/>
-      <c r="L5" s="242"/>
-      <c r="M5" s="243"/>
+      <c r="K5" s="263"/>
+      <c r="L5" s="264"/>
+      <c r="M5" s="265"/>
       <c r="N5" s="72"/>
     </row>
     <row r="6" spans="1:14" s="73" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="72"/>
-      <c r="B6" s="247"/>
-      <c r="C6" s="248"/>
-      <c r="D6" s="248"/>
-      <c r="E6" s="249"/>
-      <c r="F6" s="249"/>
-      <c r="G6" s="249"/>
-      <c r="H6" s="249"/>
+      <c r="B6" s="269"/>
+      <c r="C6" s="270"/>
+      <c r="D6" s="270"/>
+      <c r="E6" s="271"/>
+      <c r="F6" s="271"/>
+      <c r="G6" s="271"/>
+      <c r="H6" s="271"/>
       <c r="I6" s="72"/>
       <c r="J6" s="74"/>
-      <c r="K6" s="241"/>
-      <c r="L6" s="242"/>
-      <c r="M6" s="243"/>
+      <c r="K6" s="263"/>
+      <c r="L6" s="264"/>
+      <c r="M6" s="265"/>
       <c r="N6" s="72"/>
     </row>
     <row r="7" spans="1:14" s="73" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="72"/>
-      <c r="B7" s="250"/>
-      <c r="C7" s="250"/>
-      <c r="D7" s="250"/>
-      <c r="E7" s="251"/>
-      <c r="F7" s="251"/>
-      <c r="G7" s="251"/>
-      <c r="H7" s="251"/>
+      <c r="B7" s="272"/>
+      <c r="C7" s="272"/>
+      <c r="D7" s="272"/>
+      <c r="E7" s="273"/>
+      <c r="F7" s="273"/>
+      <c r="G7" s="273"/>
+      <c r="H7" s="273"/>
       <c r="I7" s="72"/>
       <c r="J7" s="72"/>
-      <c r="K7" s="241"/>
-      <c r="L7" s="242"/>
-      <c r="M7" s="243"/>
+      <c r="K7" s="263"/>
+      <c r="L7" s="264"/>
+      <c r="M7" s="265"/>
       <c r="N7" s="72"/>
     </row>
     <row r="8" spans="1:14" s="73" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="72"/>
-      <c r="B8" s="250"/>
-      <c r="C8" s="250"/>
-      <c r="D8" s="250"/>
-      <c r="E8" s="251"/>
-      <c r="F8" s="251"/>
-      <c r="G8" s="251"/>
-      <c r="H8" s="251"/>
+      <c r="B8" s="272"/>
+      <c r="C8" s="272"/>
+      <c r="D8" s="272"/>
+      <c r="E8" s="273"/>
+      <c r="F8" s="273"/>
+      <c r="G8" s="273"/>
+      <c r="H8" s="273"/>
       <c r="I8" s="72"/>
       <c r="J8" s="72"/>
-      <c r="K8" s="241"/>
-      <c r="L8" s="242"/>
-      <c r="M8" s="243"/>
+      <c r="K8" s="263"/>
+      <c r="L8" s="264"/>
+      <c r="M8" s="265"/>
       <c r="N8" s="72"/>
     </row>
     <row r="9" spans="1:14" s="73" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="72"/>
-      <c r="B9" s="252"/>
-      <c r="C9" s="252"/>
-      <c r="D9" s="252"/>
-      <c r="E9" s="253"/>
-      <c r="F9" s="253"/>
-      <c r="G9" s="253"/>
-      <c r="H9" s="253"/>
+      <c r="B9" s="274"/>
+      <c r="C9" s="274"/>
+      <c r="D9" s="274"/>
+      <c r="E9" s="250"/>
+      <c r="F9" s="250"/>
+      <c r="G9" s="250"/>
+      <c r="H9" s="250"/>
       <c r="I9" s="72"/>
       <c r="J9" s="72"/>
-      <c r="K9" s="241"/>
-      <c r="L9" s="242"/>
-      <c r="M9" s="243"/>
+      <c r="K9" s="263"/>
+      <c r="L9" s="264"/>
+      <c r="M9" s="265"/>
       <c r="N9" s="72"/>
     </row>
     <row r="10" spans="1:14" s="73" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16392,47 +16392,47 @@
       <c r="H10" s="76"/>
       <c r="I10" s="72"/>
       <c r="J10" s="72"/>
-      <c r="K10" s="241"/>
-      <c r="L10" s="242"/>
-      <c r="M10" s="243"/>
+      <c r="K10" s="263"/>
+      <c r="L10" s="264"/>
+      <c r="M10" s="265"/>
       <c r="N10" s="72"/>
     </row>
     <row r="11" spans="1:14" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="72"/>
-      <c r="B11" s="254" t="s">
+      <c r="B11" s="251" t="s">
         <v>144</v>
       </c>
-      <c r="C11" s="224"/>
-      <c r="D11" s="224"/>
-      <c r="E11" s="224"/>
-      <c r="F11" s="224"/>
-      <c r="G11" s="224"/>
-      <c r="H11" s="225"/>
+      <c r="C11" s="252"/>
+      <c r="D11" s="252"/>
+      <c r="E11" s="252"/>
+      <c r="F11" s="252"/>
+      <c r="G11" s="252"/>
+      <c r="H11" s="253"/>
       <c r="I11" s="72"/>
       <c r="J11" s="72"/>
-      <c r="K11" s="241"/>
-      <c r="L11" s="242"/>
-      <c r="M11" s="243"/>
+      <c r="K11" s="263"/>
+      <c r="L11" s="264"/>
+      <c r="M11" s="265"/>
       <c r="N11" s="72"/>
     </row>
     <row r="12" spans="1:14" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="72"/>
       <c r="B12" s="77"/>
-      <c r="C12" s="226" t="s">
+      <c r="C12" s="245" t="s">
         <v>145</v>
       </c>
-      <c r="D12" s="227"/>
-      <c r="E12" s="227"/>
-      <c r="F12" s="226" t="s">
+      <c r="D12" s="246"/>
+      <c r="E12" s="246"/>
+      <c r="F12" s="245" t="s">
         <v>146</v>
       </c>
-      <c r="G12" s="227"/>
-      <c r="H12" s="228"/>
+      <c r="G12" s="246"/>
+      <c r="H12" s="247"/>
       <c r="I12" s="72"/>
       <c r="J12" s="72"/>
-      <c r="K12" s="241"/>
-      <c r="L12" s="242"/>
-      <c r="M12" s="243"/>
+      <c r="K12" s="263"/>
+      <c r="L12" s="264"/>
+      <c r="M12" s="265"/>
       <c r="N12" s="72"/>
     </row>
     <row r="13" spans="1:14" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -16440,17 +16440,17 @@
       <c r="B13" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="235"/>
-      <c r="D13" s="236"/>
-      <c r="E13" s="237"/>
-      <c r="F13" s="232"/>
-      <c r="G13" s="233"/>
-      <c r="H13" s="234"/>
+      <c r="C13" s="226"/>
+      <c r="D13" s="227"/>
+      <c r="E13" s="228"/>
+      <c r="F13" s="242"/>
+      <c r="G13" s="243"/>
+      <c r="H13" s="244"/>
       <c r="I13" s="72"/>
       <c r="J13" s="72"/>
-      <c r="K13" s="241"/>
-      <c r="L13" s="242"/>
-      <c r="M13" s="243"/>
+      <c r="K13" s="263"/>
+      <c r="L13" s="264"/>
+      <c r="M13" s="265"/>
       <c r="N13" s="72"/>
     </row>
     <row r="14" spans="1:14" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16458,17 +16458,17 @@
       <c r="B14" s="79" t="s">
         <v>147</v>
       </c>
-      <c r="C14" s="235"/>
-      <c r="D14" s="236"/>
-      <c r="E14" s="237"/>
-      <c r="F14" s="232"/>
-      <c r="G14" s="233"/>
-      <c r="H14" s="234"/>
+      <c r="C14" s="226"/>
+      <c r="D14" s="227"/>
+      <c r="E14" s="228"/>
+      <c r="F14" s="242"/>
+      <c r="G14" s="243"/>
+      <c r="H14" s="244"/>
       <c r="I14" s="72"/>
       <c r="J14" s="80"/>
-      <c r="K14" s="241"/>
-      <c r="L14" s="242"/>
-      <c r="M14" s="243"/>
+      <c r="K14" s="263"/>
+      <c r="L14" s="264"/>
+      <c r="M14" s="265"/>
       <c r="N14" s="72"/>
     </row>
     <row r="15" spans="1:14" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -16476,17 +16476,17 @@
       <c r="B15" s="79" t="s">
         <v>148</v>
       </c>
-      <c r="C15" s="235"/>
-      <c r="D15" s="236"/>
-      <c r="E15" s="237"/>
-      <c r="F15" s="232"/>
-      <c r="G15" s="233"/>
-      <c r="H15" s="234"/>
+      <c r="C15" s="226"/>
+      <c r="D15" s="227"/>
+      <c r="E15" s="228"/>
+      <c r="F15" s="242"/>
+      <c r="G15" s="243"/>
+      <c r="H15" s="244"/>
       <c r="I15" s="72"/>
       <c r="J15" s="72"/>
-      <c r="K15" s="241"/>
-      <c r="L15" s="242"/>
-      <c r="M15" s="243"/>
+      <c r="K15" s="263"/>
+      <c r="L15" s="264"/>
+      <c r="M15" s="265"/>
       <c r="N15" s="72"/>
     </row>
     <row r="16" spans="1:14" s="73" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -16494,17 +16494,17 @@
       <c r="B16" s="79" t="s">
         <v>149</v>
       </c>
-      <c r="C16" s="235"/>
-      <c r="D16" s="236"/>
-      <c r="E16" s="237"/>
-      <c r="F16" s="232"/>
-      <c r="G16" s="233"/>
-      <c r="H16" s="234"/>
+      <c r="C16" s="226"/>
+      <c r="D16" s="227"/>
+      <c r="E16" s="228"/>
+      <c r="F16" s="242"/>
+      <c r="G16" s="243"/>
+      <c r="H16" s="244"/>
       <c r="I16" s="72"/>
       <c r="J16" s="72"/>
-      <c r="K16" s="244"/>
-      <c r="L16" s="245"/>
-      <c r="M16" s="246"/>
+      <c r="K16" s="266"/>
+      <c r="L16" s="267"/>
+      <c r="M16" s="268"/>
       <c r="N16" s="72"/>
     </row>
     <row r="17" spans="1:14" s="73" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.35">
@@ -16525,15 +16525,15 @@
     </row>
     <row r="18" spans="1:14" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="72"/>
-      <c r="B18" s="254" t="s">
+      <c r="B18" s="251" t="s">
         <v>150</v>
       </c>
-      <c r="C18" s="255"/>
-      <c r="D18" s="255"/>
-      <c r="E18" s="255"/>
-      <c r="F18" s="255"/>
-      <c r="G18" s="255"/>
-      <c r="H18" s="256"/>
+      <c r="C18" s="254"/>
+      <c r="D18" s="254"/>
+      <c r="E18" s="254"/>
+      <c r="F18" s="254"/>
+      <c r="G18" s="254"/>
+      <c r="H18" s="255"/>
       <c r="I18" s="72"/>
       <c r="J18" s="72"/>
       <c r="K18" s="72"/>
@@ -16544,16 +16544,16 @@
     <row r="19" spans="1:14" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="72"/>
       <c r="B19" s="81"/>
-      <c r="C19" s="226" t="s">
+      <c r="C19" s="245" t="s">
         <v>151</v>
       </c>
-      <c r="D19" s="227"/>
-      <c r="E19" s="227"/>
-      <c r="F19" s="226" t="s">
+      <c r="D19" s="246"/>
+      <c r="E19" s="246"/>
+      <c r="F19" s="245" t="s">
         <v>152</v>
       </c>
-      <c r="G19" s="227"/>
-      <c r="H19" s="228"/>
+      <c r="G19" s="246"/>
+      <c r="H19" s="247"/>
       <c r="I19" s="72"/>
       <c r="J19" s="72"/>
       <c r="K19" s="72"/>
@@ -16566,12 +16566,12 @@
       <c r="B20" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="235"/>
-      <c r="D20" s="236"/>
-      <c r="E20" s="237"/>
-      <c r="F20" s="232"/>
-      <c r="G20" s="233"/>
-      <c r="H20" s="234"/>
+      <c r="C20" s="226"/>
+      <c r="D20" s="227"/>
+      <c r="E20" s="228"/>
+      <c r="F20" s="242"/>
+      <c r="G20" s="243"/>
+      <c r="H20" s="244"/>
       <c r="I20" s="72"/>
       <c r="J20" s="72"/>
       <c r="K20" s="72"/>
@@ -16584,12 +16584,12 @@
       <c r="B21" s="78" t="s">
         <v>153</v>
       </c>
-      <c r="C21" s="235"/>
-      <c r="D21" s="236"/>
-      <c r="E21" s="237"/>
-      <c r="F21" s="232"/>
-      <c r="G21" s="233"/>
-      <c r="H21" s="234"/>
+      <c r="C21" s="226"/>
+      <c r="D21" s="227"/>
+      <c r="E21" s="228"/>
+      <c r="F21" s="242"/>
+      <c r="G21" s="243"/>
+      <c r="H21" s="244"/>
       <c r="I21" s="72"/>
       <c r="J21" s="72"/>
       <c r="K21" s="72"/>
@@ -16602,12 +16602,12 @@
       <c r="B22" s="78" t="s">
         <v>148</v>
       </c>
-      <c r="C22" s="235"/>
-      <c r="D22" s="236"/>
-      <c r="E22" s="237"/>
-      <c r="F22" s="232"/>
-      <c r="G22" s="233"/>
-      <c r="H22" s="234"/>
+      <c r="C22" s="226"/>
+      <c r="D22" s="227"/>
+      <c r="E22" s="228"/>
+      <c r="F22" s="242"/>
+      <c r="G22" s="243"/>
+      <c r="H22" s="244"/>
       <c r="I22" s="72"/>
       <c r="J22" s="72"/>
       <c r="K22" s="72"/>
@@ -16620,12 +16620,12 @@
       <c r="B23" s="79" t="s">
         <v>149</v>
       </c>
-      <c r="C23" s="235"/>
-      <c r="D23" s="236"/>
-      <c r="E23" s="237"/>
-      <c r="F23" s="232"/>
-      <c r="G23" s="233"/>
-      <c r="H23" s="234"/>
+      <c r="C23" s="226"/>
+      <c r="D23" s="227"/>
+      <c r="E23" s="228"/>
+      <c r="F23" s="242"/>
+      <c r="G23" s="243"/>
+      <c r="H23" s="244"/>
       <c r="I23" s="72"/>
       <c r="J23" s="72"/>
       <c r="K23" s="72"/>
@@ -16636,16 +16636,16 @@
     <row r="24" spans="1:14" s="73" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="72"/>
       <c r="B24" s="82"/>
-      <c r="C24" s="226" t="s">
+      <c r="C24" s="245" t="s">
         <v>154</v>
       </c>
-      <c r="D24" s="227"/>
-      <c r="E24" s="227"/>
-      <c r="F24" s="226" t="s">
+      <c r="D24" s="246"/>
+      <c r="E24" s="246"/>
+      <c r="F24" s="245" t="s">
         <v>155</v>
       </c>
-      <c r="G24" s="227"/>
-      <c r="H24" s="228"/>
+      <c r="G24" s="246"/>
+      <c r="H24" s="247"/>
       <c r="I24" s="72"/>
       <c r="J24" s="72"/>
       <c r="K24" s="72"/>
@@ -16658,12 +16658,12 @@
       <c r="B25" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="235"/>
-      <c r="D25" s="236"/>
-      <c r="E25" s="237"/>
-      <c r="F25" s="232"/>
-      <c r="G25" s="233"/>
-      <c r="H25" s="234"/>
+      <c r="C25" s="226"/>
+      <c r="D25" s="227"/>
+      <c r="E25" s="228"/>
+      <c r="F25" s="242"/>
+      <c r="G25" s="243"/>
+      <c r="H25" s="244"/>
       <c r="I25" s="72"/>
       <c r="J25" s="72"/>
       <c r="K25" s="83" t="s">
@@ -16678,12 +16678,12 @@
       <c r="B26" s="78" t="s">
         <v>153</v>
       </c>
-      <c r="C26" s="235"/>
-      <c r="D26" s="236"/>
-      <c r="E26" s="237"/>
-      <c r="F26" s="232"/>
-      <c r="G26" s="233"/>
-      <c r="H26" s="234"/>
+      <c r="C26" s="226"/>
+      <c r="D26" s="227"/>
+      <c r="E26" s="228"/>
+      <c r="F26" s="242"/>
+      <c r="G26" s="243"/>
+      <c r="H26" s="244"/>
       <c r="I26" s="72"/>
       <c r="J26" s="72"/>
       <c r="K26" s="85" t="s">
@@ -16698,12 +16698,12 @@
       <c r="B27" s="78" t="s">
         <v>148</v>
       </c>
-      <c r="C27" s="235"/>
-      <c r="D27" s="236"/>
-      <c r="E27" s="237"/>
-      <c r="F27" s="232"/>
-      <c r="G27" s="233"/>
-      <c r="H27" s="234"/>
+      <c r="C27" s="226"/>
+      <c r="D27" s="227"/>
+      <c r="E27" s="228"/>
+      <c r="F27" s="242"/>
+      <c r="G27" s="243"/>
+      <c r="H27" s="244"/>
       <c r="I27" s="72"/>
       <c r="J27" s="72"/>
       <c r="K27" s="85" t="s">
@@ -16718,12 +16718,12 @@
       <c r="B28" s="79" t="s">
         <v>149</v>
       </c>
-      <c r="C28" s="235"/>
-      <c r="D28" s="236"/>
-      <c r="E28" s="237"/>
-      <c r="F28" s="232"/>
-      <c r="G28" s="233"/>
-      <c r="H28" s="234"/>
+      <c r="C28" s="226"/>
+      <c r="D28" s="227"/>
+      <c r="E28" s="228"/>
+      <c r="F28" s="242"/>
+      <c r="G28" s="243"/>
+      <c r="H28" s="244"/>
       <c r="I28" s="72"/>
       <c r="J28" s="72"/>
       <c r="K28" s="87" t="s">
@@ -16738,9 +16738,9 @@
       <c r="B29" s="78" t="s">
         <v>160</v>
       </c>
-      <c r="C29" s="257"/>
-      <c r="D29" s="258"/>
-      <c r="E29" s="259"/>
+      <c r="C29" s="233"/>
+      <c r="D29" s="248"/>
+      <c r="E29" s="249"/>
       <c r="F29" s="64"/>
       <c r="G29" s="90"/>
       <c r="H29" s="90"/>
@@ -16754,16 +16754,16 @@
     <row r="30" spans="1:14" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="72"/>
       <c r="B30" s="82"/>
-      <c r="C30" s="226" t="s">
+      <c r="C30" s="245" t="s">
         <v>161</v>
       </c>
-      <c r="D30" s="227"/>
-      <c r="E30" s="228"/>
-      <c r="F30" s="226" t="s">
+      <c r="D30" s="246"/>
+      <c r="E30" s="247"/>
+      <c r="F30" s="245" t="s">
         <v>201</v>
       </c>
-      <c r="G30" s="227"/>
-      <c r="H30" s="228"/>
+      <c r="G30" s="246"/>
+      <c r="H30" s="247"/>
       <c r="I30" s="72"/>
       <c r="J30" s="72"/>
       <c r="K30" s="91"/>
@@ -16776,12 +16776,12 @@
       <c r="B31" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="235"/>
-      <c r="D31" s="236"/>
-      <c r="E31" s="237"/>
-      <c r="F31" s="263"/>
-      <c r="G31" s="264"/>
-      <c r="H31" s="265"/>
+      <c r="C31" s="226"/>
+      <c r="D31" s="227"/>
+      <c r="E31" s="228"/>
+      <c r="F31" s="229"/>
+      <c r="G31" s="230"/>
+      <c r="H31" s="231"/>
       <c r="I31" s="92"/>
       <c r="J31" s="92"/>
       <c r="K31" s="69"/>
@@ -16794,12 +16794,12 @@
       <c r="B32" s="78" t="s">
         <v>153</v>
       </c>
-      <c r="C32" s="235"/>
-      <c r="D32" s="236"/>
-      <c r="E32" s="237"/>
-      <c r="F32" s="263"/>
-      <c r="G32" s="264"/>
-      <c r="H32" s="265"/>
+      <c r="C32" s="226"/>
+      <c r="D32" s="227"/>
+      <c r="E32" s="228"/>
+      <c r="F32" s="229"/>
+      <c r="G32" s="230"/>
+      <c r="H32" s="231"/>
       <c r="I32" s="92"/>
       <c r="J32" s="92"/>
       <c r="K32" s="69"/>
@@ -16812,12 +16812,12 @@
       <c r="B33" s="78" t="s">
         <v>148</v>
       </c>
-      <c r="C33" s="235"/>
-      <c r="D33" s="236"/>
-      <c r="E33" s="237"/>
-      <c r="F33" s="263"/>
-      <c r="G33" s="264"/>
-      <c r="H33" s="265"/>
+      <c r="C33" s="226"/>
+      <c r="D33" s="227"/>
+      <c r="E33" s="228"/>
+      <c r="F33" s="229"/>
+      <c r="G33" s="230"/>
+      <c r="H33" s="231"/>
       <c r="I33" s="92"/>
       <c r="J33" s="92"/>
       <c r="K33" s="69"/>
@@ -16830,12 +16830,12 @@
       <c r="B34" s="79" t="s">
         <v>149</v>
       </c>
-      <c r="C34" s="235"/>
-      <c r="D34" s="236"/>
-      <c r="E34" s="237"/>
-      <c r="F34" s="266"/>
-      <c r="G34" s="264"/>
-      <c r="H34" s="265"/>
+      <c r="C34" s="226"/>
+      <c r="D34" s="227"/>
+      <c r="E34" s="228"/>
+      <c r="F34" s="232"/>
+      <c r="G34" s="230"/>
+      <c r="H34" s="231"/>
       <c r="I34" s="92"/>
       <c r="J34" s="92"/>
       <c r="K34" s="69"/>
@@ -16848,9 +16848,9 @@
       <c r="B35" s="79" t="s">
         <v>162</v>
       </c>
-      <c r="C35" s="257"/>
-      <c r="D35" s="267"/>
-      <c r="E35" s="268"/>
+      <c r="C35" s="233"/>
+      <c r="D35" s="234"/>
+      <c r="E35" s="235"/>
       <c r="F35" s="93"/>
       <c r="G35" s="93"/>
       <c r="H35" s="93"/>
@@ -16879,12 +16879,12 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="92"/>
-      <c r="B37" s="269" t="s">
+      <c r="B37" s="236" t="s">
         <v>163</v>
       </c>
-      <c r="C37" s="270"/>
-      <c r="D37" s="270"/>
-      <c r="E37" s="271"/>
+      <c r="C37" s="237"/>
+      <c r="D37" s="237"/>
+      <c r="E37" s="238"/>
       <c r="F37" s="93"/>
       <c r="G37" s="93"/>
       <c r="H37" s="93"/>
@@ -16897,11 +16897,11 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="92"/>
-      <c r="B38" s="272" t="s">
+      <c r="B38" s="239" t="s">
         <v>164</v>
       </c>
-      <c r="C38" s="273"/>
-      <c r="D38" s="274"/>
+      <c r="C38" s="240"/>
+      <c r="D38" s="241"/>
       <c r="E38" s="94"/>
       <c r="F38" s="93"/>
       <c r="G38" s="93"/>
@@ -16915,11 +16915,11 @@
     </row>
     <row r="39" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="92"/>
-      <c r="B39" s="260" t="s">
+      <c r="B39" s="223" t="s">
         <v>165</v>
       </c>
-      <c r="C39" s="261"/>
-      <c r="D39" s="262"/>
+      <c r="C39" s="224"/>
+      <c r="D39" s="225"/>
       <c r="E39" s="95"/>
       <c r="F39" s="93"/>
       <c r="G39" s="93"/>
@@ -16949,38 +16949,22 @@
     </row>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="K4:M16"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="B9:D9"/>
     <mergeCell ref="E9:H9"/>
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="C12:E12"/>
@@ -16997,22 +16981,38 @@
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="B18:H18"/>
     <mergeCell ref="C19:E19"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="K4:M16"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B38:D38"/>
   </mergeCells>
   <conditionalFormatting sqref="B4 E4">
     <cfRule type="expression" dxfId="162" priority="7">
@@ -17610,7 +17610,7 @@
   </sheetPr>
   <dimension ref="S3:W15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
@@ -20797,60 +20797,60 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="E2" s="286" t="s">
+      <c r="E2" s="300" t="s">
         <v>405</v>
       </c>
-      <c r="F2" s="286"/>
-      <c r="G2" s="286"/>
-      <c r="H2" s="286"/>
-      <c r="I2" s="286"/>
-      <c r="J2" s="286"/>
-      <c r="K2" s="286"/>
-      <c r="L2" s="286"/>
-      <c r="M2" s="286"/>
-      <c r="N2" s="286"/>
-      <c r="O2" s="286"/>
-      <c r="P2" s="286"/>
+      <c r="F2" s="300"/>
+      <c r="G2" s="300"/>
+      <c r="H2" s="300"/>
+      <c r="I2" s="300"/>
+      <c r="J2" s="300"/>
+      <c r="K2" s="300"/>
+      <c r="L2" s="300"/>
+      <c r="M2" s="300"/>
+      <c r="N2" s="300"/>
+      <c r="O2" s="300"/>
+      <c r="P2" s="300"/>
       <c r="X2" s="137"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A3" s="292" t="s">
+      <c r="A3" s="291" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="293"/>
+      <c r="B3" s="292"/>
       <c r="C3" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="E3" s="294" t="s">
+      <c r="E3" s="304" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="289"/>
-      <c r="G3" s="289" t="s">
+      <c r="F3" s="302"/>
+      <c r="G3" s="302" t="s">
         <v>49</v>
       </c>
-      <c r="H3" s="289"/>
-      <c r="I3" s="289" t="s">
+      <c r="H3" s="302"/>
+      <c r="I3" s="302" t="s">
         <v>44</v>
       </c>
-      <c r="J3" s="289"/>
-      <c r="K3" s="295" t="s">
+      <c r="J3" s="302"/>
+      <c r="K3" s="305" t="s">
         <v>298</v>
       </c>
-      <c r="L3" s="296"/>
-      <c r="M3" s="297"/>
+      <c r="L3" s="306"/>
+      <c r="M3" s="307"/>
       <c r="N3" s="150"/>
-      <c r="O3" s="289" t="s">
+      <c r="O3" s="302" t="s">
         <v>45</v>
       </c>
-      <c r="P3" s="290"/>
-      <c r="R3" s="287" t="s">
+      <c r="P3" s="303"/>
+      <c r="R3" s="301" t="s">
         <v>54</v>
       </c>
-      <c r="S3" s="287"/>
-      <c r="T3" s="288"/>
-      <c r="U3" s="288"/>
-      <c r="V3" s="288"/>
-      <c r="W3" s="288"/>
+      <c r="S3" s="301"/>
+      <c r="T3" s="295"/>
+      <c r="U3" s="295"/>
+      <c r="V3" s="295"/>
+      <c r="W3" s="295"/>
       <c r="X3" s="137"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.35">
@@ -20899,14 +20899,14 @@
       <c r="P4" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="R4" s="291" t="s">
+      <c r="R4" s="296" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="291"/>
-      <c r="T4" s="288"/>
-      <c r="U4" s="288"/>
-      <c r="V4" s="288"/>
-      <c r="W4" s="288"/>
+      <c r="S4" s="296"/>
+      <c r="T4" s="295"/>
+      <c r="U4" s="295"/>
+      <c r="V4" s="295"/>
+      <c r="W4" s="295"/>
       <c r="X4" s="137"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.35">
@@ -20956,14 +20956,14 @@
       <c r="P5" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R5" s="287" t="s">
+      <c r="R5" s="301" t="s">
         <v>42</v>
       </c>
-      <c r="S5" s="287"/>
-      <c r="T5" s="288"/>
-      <c r="U5" s="288"/>
-      <c r="V5" s="288"/>
-      <c r="W5" s="288"/>
+      <c r="S5" s="301"/>
+      <c r="T5" s="295"/>
+      <c r="U5" s="295"/>
+      <c r="V5" s="295"/>
+      <c r="W5" s="295"/>
       <c r="X5" s="137"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.35">
@@ -21013,17 +21013,17 @@
       <c r="P6" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R6" s="291" t="s">
+      <c r="R6" s="296" t="s">
         <v>71</v>
       </c>
-      <c r="S6" s="291"/>
-      <c r="T6" s="288" t="str">
+      <c r="S6" s="296"/>
+      <c r="T6" s="295" t="str">
         <f>S3048_FW</f>
         <v>fw: 9.11(0.0)</v>
       </c>
-      <c r="U6" s="288"/>
-      <c r="V6" s="288"/>
-      <c r="W6" s="288"/>
+      <c r="U6" s="295"/>
+      <c r="V6" s="295"/>
+      <c r="W6" s="295"/>
       <c r="X6" s="137"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.35">
@@ -21122,16 +21122,16 @@
       <c r="P8" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R8" s="301" t="s">
+      <c r="R8" s="293" t="s">
         <v>167</v>
       </c>
-      <c r="S8" s="301"/>
-      <c r="T8" s="301"/>
-      <c r="U8" s="302" t="s">
+      <c r="S8" s="293"/>
+      <c r="T8" s="293"/>
+      <c r="U8" s="294" t="s">
         <v>289</v>
       </c>
-      <c r="V8" s="302"/>
-      <c r="W8" s="302"/>
+      <c r="V8" s="294"/>
+      <c r="W8" s="294"/>
       <c r="X8" s="137"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.35">
@@ -21181,14 +21181,14 @@
       <c r="P9" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R9" s="303" t="s">
+      <c r="R9" s="297" t="s">
         <v>55</v>
       </c>
-      <c r="S9" s="303"/>
-      <c r="T9" s="303"/>
-      <c r="U9" s="288"/>
-      <c r="V9" s="288"/>
-      <c r="W9" s="288"/>
+      <c r="S9" s="297"/>
+      <c r="T9" s="297"/>
+      <c r="U9" s="295"/>
+      <c r="V9" s="295"/>
+      <c r="W9" s="295"/>
       <c r="X9" s="137"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.35">
@@ -21238,16 +21238,16 @@
       <c r="P10" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R10" s="304" t="s">
+      <c r="R10" s="298" t="s">
         <v>56</v>
       </c>
-      <c r="S10" s="304"/>
-      <c r="T10" s="304"/>
-      <c r="U10" s="288">
+      <c r="S10" s="298"/>
+      <c r="T10" s="298"/>
+      <c r="U10" s="295">
         <v>24576</v>
       </c>
-      <c r="V10" s="288"/>
-      <c r="W10" s="288"/>
+      <c r="V10" s="295"/>
+      <c r="W10" s="295"/>
       <c r="X10" s="137"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.35">
@@ -21344,16 +21344,16 @@
       <c r="P12" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R12" s="301" t="s">
+      <c r="R12" s="293" t="s">
         <v>58</v>
       </c>
-      <c r="S12" s="301"/>
-      <c r="T12" s="301"/>
-      <c r="U12" s="302" t="s">
+      <c r="S12" s="293"/>
+      <c r="T12" s="293"/>
+      <c r="U12" s="294" t="s">
         <v>290</v>
       </c>
-      <c r="V12" s="302"/>
-      <c r="W12" s="302"/>
+      <c r="V12" s="294"/>
+      <c r="W12" s="294"/>
       <c r="X12" s="137"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.35">
@@ -21403,10 +21403,10 @@
       <c r="X13" s="137"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A14" s="294" t="s">
+      <c r="A14" s="304" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="290"/>
+      <c r="B14" s="303"/>
       <c r="C14" s="34"/>
       <c r="E14" s="36" t="s">
         <v>328</v>
@@ -21441,14 +21441,14 @@
       <c r="P14" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R14" s="298" t="s">
+      <c r="R14" s="308" t="s">
         <v>70</v>
       </c>
-      <c r="S14" s="299"/>
-      <c r="T14" s="299"/>
-      <c r="U14" s="299"/>
-      <c r="V14" s="299"/>
-      <c r="W14" s="300"/>
+      <c r="S14" s="309"/>
+      <c r="T14" s="309"/>
+      <c r="U14" s="309"/>
+      <c r="V14" s="309"/>
+      <c r="W14" s="310"/>
       <c r="X14" s="137"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.35">
@@ -21494,12 +21494,12 @@
       <c r="P15" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R15" s="305"/>
-      <c r="S15" s="306"/>
-      <c r="T15" s="306"/>
-      <c r="U15" s="306"/>
-      <c r="V15" s="306"/>
-      <c r="W15" s="307"/>
+      <c r="R15" s="285"/>
+      <c r="S15" s="286"/>
+      <c r="T15" s="286"/>
+      <c r="U15" s="286"/>
+      <c r="V15" s="286"/>
+      <c r="W15" s="287"/>
       <c r="X15" s="137"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.35">
@@ -21545,12 +21545,12 @@
       <c r="P16" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R16" s="308"/>
-      <c r="S16" s="309"/>
-      <c r="T16" s="309"/>
-      <c r="U16" s="309"/>
-      <c r="V16" s="309"/>
-      <c r="W16" s="310"/>
+      <c r="R16" s="288"/>
+      <c r="S16" s="289"/>
+      <c r="T16" s="289"/>
+      <c r="U16" s="289"/>
+      <c r="V16" s="289"/>
+      <c r="W16" s="290"/>
       <c r="X16" s="137"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.35">
@@ -21599,12 +21599,12 @@
       <c r="P17" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R17" s="305"/>
-      <c r="S17" s="306"/>
-      <c r="T17" s="306"/>
-      <c r="U17" s="306"/>
-      <c r="V17" s="306"/>
-      <c r="W17" s="307"/>
+      <c r="R17" s="285"/>
+      <c r="S17" s="286"/>
+      <c r="T17" s="286"/>
+      <c r="U17" s="286"/>
+      <c r="V17" s="286"/>
+      <c r="W17" s="287"/>
       <c r="X17" s="137"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.35">
@@ -21653,12 +21653,12 @@
       <c r="P18" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R18" s="308"/>
-      <c r="S18" s="309"/>
-      <c r="T18" s="309"/>
-      <c r="U18" s="309"/>
-      <c r="V18" s="309"/>
-      <c r="W18" s="310"/>
+      <c r="R18" s="288"/>
+      <c r="S18" s="289"/>
+      <c r="T18" s="289"/>
+      <c r="U18" s="289"/>
+      <c r="V18" s="289"/>
+      <c r="W18" s="290"/>
       <c r="X18" s="137"/>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.35">
@@ -21921,10 +21921,10 @@
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A25" s="292" t="s">
+      <c r="A25" s="291" t="s">
         <v>65</v>
       </c>
-      <c r="B25" s="293"/>
+      <c r="B25" s="292"/>
       <c r="C25" s="34"/>
       <c r="E25" s="36" t="s">
         <v>339</v>
@@ -22162,11 +22162,11 @@
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A31" s="285" t="s">
+      <c r="A31" s="299" t="s">
         <v>400</v>
       </c>
-      <c r="B31" s="285"/>
-      <c r="C31" s="285"/>
+      <c r="B31" s="299"/>
+      <c r="C31" s="299"/>
       <c r="E31" s="36" t="s">
         <v>345</v>
       </c>
@@ -22202,9 +22202,9 @@
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A32" s="285"/>
-      <c r="B32" s="285"/>
-      <c r="C32" s="285"/>
+      <c r="A32" s="299"/>
+      <c r="B32" s="299"/>
+      <c r="C32" s="299"/>
       <c r="E32" s="36" t="s">
         <v>346</v>
       </c>
@@ -22242,9 +22242,9 @@
       </c>
     </row>
     <row r="33" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="285"/>
-      <c r="B33" s="285"/>
-      <c r="C33" s="285"/>
+      <c r="A33" s="299"/>
+      <c r="B33" s="299"/>
+      <c r="C33" s="299"/>
       <c r="E33" s="36" t="s">
         <v>347</v>
       </c>
@@ -23052,21 +23052,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="R15:W15"/>
-    <mergeCell ref="R16:W16"/>
-    <mergeCell ref="R17:W17"/>
-    <mergeCell ref="R18:W18"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="R12:T12"/>
-    <mergeCell ref="U12:W12"/>
-    <mergeCell ref="T6:W6"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="U8:W8"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="R9:T9"/>
-    <mergeCell ref="U9:W9"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="U10:W10"/>
     <mergeCell ref="A31:C33"/>
     <mergeCell ref="E2:P2"/>
     <mergeCell ref="R5:S5"/>
@@ -23083,6 +23068,21 @@
     <mergeCell ref="K3:M3"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="R14:W14"/>
+    <mergeCell ref="R12:T12"/>
+    <mergeCell ref="U12:W12"/>
+    <mergeCell ref="T6:W6"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="U8:W8"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="U9:W9"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="U10:W10"/>
+    <mergeCell ref="R15:W15"/>
+    <mergeCell ref="R16:W16"/>
+    <mergeCell ref="R17:W17"/>
+    <mergeCell ref="R18:W18"/>
+    <mergeCell ref="A25:B25"/>
   </mergeCells>
   <conditionalFormatting sqref="F37:F43 F46:F48">
     <cfRule type="expression" dxfId="90" priority="6" stopIfTrue="1">
@@ -23176,56 +23176,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="E1" s="286" t="s">
+      <c r="E1" s="300" t="s">
         <v>405</v>
       </c>
-      <c r="F1" s="286"/>
-      <c r="G1" s="286"/>
-      <c r="H1" s="286"/>
-      <c r="I1" s="286"/>
-      <c r="J1" s="286"/>
-      <c r="K1" s="286"/>
-      <c r="L1" s="286"/>
-      <c r="M1" s="286"/>
-      <c r="N1" s="286"/>
-      <c r="O1" s="286"/>
-      <c r="P1" s="286"/>
-      <c r="Q1" s="286"/>
+      <c r="F1" s="300"/>
+      <c r="G1" s="300"/>
+      <c r="H1" s="300"/>
+      <c r="I1" s="300"/>
+      <c r="J1" s="300"/>
+      <c r="K1" s="300"/>
+      <c r="L1" s="300"/>
+      <c r="M1" s="300"/>
+      <c r="N1" s="300"/>
+      <c r="O1" s="300"/>
+      <c r="P1" s="300"/>
+      <c r="Q1" s="300"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
-      <c r="E2" s="294" t="s">
+      <c r="E2" s="304" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="289"/>
-      <c r="G2" s="289" t="s">
+      <c r="F2" s="302"/>
+      <c r="G2" s="302" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="289"/>
-      <c r="I2" s="289" t="s">
+      <c r="H2" s="302"/>
+      <c r="I2" s="302" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="289"/>
+      <c r="J2" s="302"/>
       <c r="K2" s="151"/>
-      <c r="L2" s="295" t="s">
+      <c r="L2" s="305" t="s">
         <v>298</v>
       </c>
-      <c r="M2" s="296"/>
-      <c r="N2" s="296"/>
-      <c r="O2" s="297"/>
-      <c r="P2" s="289" t="s">
+      <c r="M2" s="306"/>
+      <c r="N2" s="306"/>
+      <c r="O2" s="307"/>
+      <c r="P2" s="302" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="290"/>
+      <c r="Q2" s="303"/>
       <c r="Z2" s="137"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A3" s="292" t="s">
+      <c r="A3" s="291" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="293"/>
+      <c r="B3" s="292"/>
       <c r="C3" s="34" t="s">
         <v>222</v>
       </c>
@@ -23268,14 +23268,14 @@
       <c r="Q3" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="T3" s="287" t="s">
+      <c r="T3" s="301" t="s">
         <v>54</v>
       </c>
-      <c r="U3" s="287"/>
-      <c r="V3" s="288"/>
-      <c r="W3" s="288"/>
-      <c r="X3" s="288"/>
-      <c r="Y3" s="288"/>
+      <c r="U3" s="301"/>
+      <c r="V3" s="295"/>
+      <c r="W3" s="295"/>
+      <c r="X3" s="295"/>
+      <c r="Y3" s="295"/>
       <c r="Z3" s="139"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.35">
@@ -23328,14 +23328,14 @@
       <c r="Q4" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="T4" s="291" t="s">
+      <c r="T4" s="296" t="s">
         <v>53</v>
       </c>
-      <c r="U4" s="291"/>
-      <c r="V4" s="288"/>
-      <c r="W4" s="288"/>
-      <c r="X4" s="288"/>
-      <c r="Y4" s="288"/>
+      <c r="U4" s="296"/>
+      <c r="V4" s="295"/>
+      <c r="W4" s="295"/>
+      <c r="X4" s="295"/>
+      <c r="Y4" s="295"/>
       <c r="Z4" s="139"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.35">
@@ -23390,14 +23390,14 @@
       <c r="Q5" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="T5" s="287" t="s">
+      <c r="T5" s="301" t="s">
         <v>42</v>
       </c>
-      <c r="U5" s="287"/>
-      <c r="V5" s="288"/>
-      <c r="W5" s="288"/>
-      <c r="X5" s="288"/>
-      <c r="Y5" s="288"/>
+      <c r="U5" s="301"/>
+      <c r="V5" s="295"/>
+      <c r="W5" s="295"/>
+      <c r="X5" s="295"/>
+      <c r="Y5" s="295"/>
       <c r="Z5" s="139"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.35">
@@ -23452,17 +23452,17 @@
       <c r="Q6" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="T6" s="291" t="s">
+      <c r="T6" s="296" t="s">
         <v>71</v>
       </c>
-      <c r="U6" s="291"/>
-      <c r="V6" s="288" t="str">
+      <c r="U6" s="296"/>
+      <c r="V6" s="295" t="str">
         <f>S4048_1_FW</f>
         <v>fw: 9.11(0.0P2)</v>
       </c>
-      <c r="W6" s="288"/>
-      <c r="X6" s="288"/>
-      <c r="Y6" s="288"/>
+      <c r="W6" s="295"/>
+      <c r="X6" s="295"/>
+      <c r="Y6" s="295"/>
       <c r="Z6" s="139"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.35">
@@ -23571,16 +23571,16 @@
       <c r="Q8" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="T8" s="301" t="s">
+      <c r="T8" s="293" t="s">
         <v>167</v>
       </c>
-      <c r="U8" s="301"/>
-      <c r="V8" s="301"/>
-      <c r="W8" s="302" t="s">
+      <c r="U8" s="293"/>
+      <c r="V8" s="293"/>
+      <c r="W8" s="294" t="s">
         <v>289</v>
       </c>
-      <c r="X8" s="302"/>
-      <c r="Y8" s="302"/>
+      <c r="X8" s="294"/>
+      <c r="Y8" s="294"/>
       <c r="Z8" s="139"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.35">
@@ -23635,14 +23635,14 @@
       <c r="Q9" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="T9" s="303" t="s">
+      <c r="T9" s="297" t="s">
         <v>55</v>
       </c>
-      <c r="U9" s="303"/>
-      <c r="V9" s="303"/>
-      <c r="W9" s="288"/>
-      <c r="X9" s="288"/>
-      <c r="Y9" s="288"/>
+      <c r="U9" s="297"/>
+      <c r="V9" s="297"/>
+      <c r="W9" s="295"/>
+      <c r="X9" s="295"/>
+      <c r="Y9" s="295"/>
       <c r="Z9" s="139"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.35">
@@ -23697,16 +23697,16 @@
       <c r="Q10" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="T10" s="304" t="s">
+      <c r="T10" s="298" t="s">
         <v>56</v>
       </c>
-      <c r="U10" s="304"/>
-      <c r="V10" s="304"/>
-      <c r="W10" s="288">
+      <c r="U10" s="298"/>
+      <c r="V10" s="298"/>
+      <c r="W10" s="295">
         <v>16384</v>
       </c>
-      <c r="X10" s="288"/>
-      <c r="Y10" s="288"/>
+      <c r="X10" s="295"/>
+      <c r="Y10" s="295"/>
       <c r="Z10" s="139"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.35">
@@ -23781,14 +23781,14 @@
       <c r="O12" s="130"/>
       <c r="P12" s="48"/>
       <c r="Q12" s="61"/>
-      <c r="T12" s="317" t="s">
+      <c r="T12" s="312" t="s">
         <v>59</v>
       </c>
-      <c r="U12" s="318"/>
-      <c r="V12" s="319"/>
-      <c r="W12" s="320"/>
-      <c r="X12" s="321"/>
-      <c r="Y12" s="322"/>
+      <c r="U12" s="313"/>
+      <c r="V12" s="314"/>
+      <c r="W12" s="315"/>
+      <c r="X12" s="316"/>
+      <c r="Y12" s="317"/>
       <c r="Z12" s="139"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.35">
@@ -23825,16 +23825,16 @@
       <c r="O13" s="130"/>
       <c r="P13" s="48"/>
       <c r="Q13" s="61"/>
-      <c r="T13" s="314" t="s">
+      <c r="T13" s="318" t="s">
         <v>60</v>
       </c>
-      <c r="U13" s="315"/>
-      <c r="V13" s="316"/>
-      <c r="W13" s="311">
+      <c r="U13" s="319"/>
+      <c r="V13" s="320"/>
+      <c r="W13" s="321">
         <v>1</v>
       </c>
-      <c r="X13" s="312"/>
-      <c r="Y13" s="313"/>
+      <c r="X13" s="322"/>
+      <c r="Y13" s="323"/>
       <c r="Z13" s="139"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.35">
@@ -23864,23 +23864,23 @@
       <c r="O14" s="130"/>
       <c r="P14" s="48"/>
       <c r="Q14" s="61"/>
-      <c r="T14" s="314" t="s">
+      <c r="T14" s="318" t="s">
         <v>166</v>
       </c>
-      <c r="U14" s="315"/>
-      <c r="V14" s="316"/>
-      <c r="W14" s="320">
+      <c r="U14" s="319"/>
+      <c r="V14" s="320"/>
+      <c r="W14" s="315">
         <v>1</v>
       </c>
-      <c r="X14" s="321"/>
-      <c r="Y14" s="322"/>
+      <c r="X14" s="316"/>
+      <c r="Y14" s="317"/>
       <c r="Z14" s="139"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A15" s="294" t="s">
+      <c r="A15" s="304" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="290"/>
+      <c r="B15" s="303"/>
       <c r="C15" s="36"/>
       <c r="E15" s="36" t="s">
         <v>241</v>
@@ -23922,16 +23922,16 @@
       <c r="Q15" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="T15" s="317" t="s">
+      <c r="T15" s="312" t="s">
         <v>67</v>
       </c>
-      <c r="U15" s="318"/>
-      <c r="V15" s="319"/>
-      <c r="W15" s="320">
+      <c r="U15" s="313"/>
+      <c r="V15" s="314"/>
+      <c r="W15" s="315">
         <v>0</v>
       </c>
-      <c r="X15" s="321"/>
-      <c r="Y15" s="322"/>
+      <c r="X15" s="316"/>
+      <c r="Y15" s="317"/>
       <c r="Z15" s="139"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.35">
@@ -24032,14 +24032,14 @@
       <c r="Q17" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="T17" s="298" t="s">
+      <c r="T17" s="308" t="s">
         <v>70</v>
       </c>
-      <c r="U17" s="299"/>
-      <c r="V17" s="299"/>
-      <c r="W17" s="299"/>
-      <c r="X17" s="299"/>
-      <c r="Y17" s="300"/>
+      <c r="U17" s="309"/>
+      <c r="V17" s="309"/>
+      <c r="W17" s="309"/>
+      <c r="X17" s="309"/>
+      <c r="Y17" s="310"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A18" s="39">
@@ -24074,12 +24074,12 @@
       <c r="Q18" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="T18" s="305"/>
-      <c r="U18" s="306"/>
-      <c r="V18" s="306"/>
-      <c r="W18" s="306"/>
-      <c r="X18" s="306"/>
-      <c r="Y18" s="307"/>
+      <c r="T18" s="285"/>
+      <c r="U18" s="286"/>
+      <c r="V18" s="286"/>
+      <c r="W18" s="286"/>
+      <c r="X18" s="286"/>
+      <c r="Y18" s="287"/>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A19" s="39">
@@ -24114,12 +24114,12 @@
       <c r="Q19" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="T19" s="308"/>
-      <c r="U19" s="309"/>
-      <c r="V19" s="309"/>
-      <c r="W19" s="309"/>
-      <c r="X19" s="309"/>
-      <c r="Y19" s="310"/>
+      <c r="T19" s="288"/>
+      <c r="U19" s="289"/>
+      <c r="V19" s="289"/>
+      <c r="W19" s="289"/>
+      <c r="X19" s="289"/>
+      <c r="Y19" s="290"/>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A20" s="39">
@@ -24148,12 +24148,12 @@
       <c r="Q20" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="T20" s="305"/>
-      <c r="U20" s="306"/>
-      <c r="V20" s="306"/>
-      <c r="W20" s="306"/>
-      <c r="X20" s="306"/>
-      <c r="Y20" s="307"/>
+      <c r="T20" s="285"/>
+      <c r="U20" s="286"/>
+      <c r="V20" s="286"/>
+      <c r="W20" s="286"/>
+      <c r="X20" s="286"/>
+      <c r="Y20" s="287"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A21" s="39">
@@ -24182,12 +24182,12 @@
       <c r="Q21" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="T21" s="308"/>
-      <c r="U21" s="309"/>
-      <c r="V21" s="309"/>
-      <c r="W21" s="309"/>
-      <c r="X21" s="309"/>
-      <c r="Y21" s="310"/>
+      <c r="T21" s="288"/>
+      <c r="U21" s="289"/>
+      <c r="V21" s="289"/>
+      <c r="W21" s="289"/>
+      <c r="X21" s="289"/>
+      <c r="Y21" s="290"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A22" s="39">
@@ -24300,10 +24300,10 @@
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A26" s="323" t="s">
+      <c r="A26" s="311" t="s">
         <v>401</v>
       </c>
-      <c r="B26" s="323"/>
+      <c r="B26" s="311"/>
       <c r="C26" s="36"/>
       <c r="E26" s="36" t="s">
         <v>252</v>
@@ -24328,8 +24328,8 @@
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A27" s="323"/>
-      <c r="B27" s="323"/>
+      <c r="A27" s="311"/>
+      <c r="B27" s="311"/>
       <c r="C27" s="36"/>
       <c r="E27" s="36" t="s">
         <v>253</v>
@@ -24354,10 +24354,10 @@
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A28" s="292" t="s">
+      <c r="A28" s="291" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="293"/>
+      <c r="B28" s="292"/>
       <c r="C28" s="36"/>
       <c r="E28" s="36" t="s">
         <v>254</v>
@@ -24582,9 +24582,9 @@
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A33" s="285"/>
-      <c r="B33" s="285"/>
-      <c r="C33" s="285"/>
+      <c r="A33" s="299"/>
+      <c r="B33" s="299"/>
+      <c r="C33" s="299"/>
       <c r="E33" s="36" t="s">
         <v>259</v>
       </c>
@@ -24627,9 +24627,9 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A34" s="285"/>
-      <c r="B34" s="285"/>
-      <c r="C34" s="285"/>
+      <c r="A34" s="299"/>
+      <c r="B34" s="299"/>
+      <c r="C34" s="299"/>
       <c r="E34" s="36" t="s">
         <v>260</v>
       </c>
@@ -24672,9 +24672,9 @@
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A35" s="285"/>
-      <c r="B35" s="285"/>
-      <c r="C35" s="285"/>
+      <c r="A35" s="299"/>
+      <c r="B35" s="299"/>
+      <c r="C35" s="299"/>
       <c r="E35" s="36" t="s">
         <v>261</v>
       </c>
@@ -25406,28 +25406,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="E1:Q1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A26:B27"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="T15:V15"/>
-    <mergeCell ref="W15:Y15"/>
-    <mergeCell ref="T17:Y17"/>
-    <mergeCell ref="T18:Y18"/>
-    <mergeCell ref="W14:Y14"/>
-    <mergeCell ref="T14:V14"/>
-    <mergeCell ref="T8:V8"/>
-    <mergeCell ref="W8:Y8"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="T10:V10"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="V6:Y6"/>
     <mergeCell ref="A33:C35"/>
     <mergeCell ref="T20:Y20"/>
     <mergeCell ref="T21:Y21"/>
@@ -25444,6 +25422,28 @@
     <mergeCell ref="W12:Y12"/>
     <mergeCell ref="W10:Y10"/>
     <mergeCell ref="T19:Y19"/>
+    <mergeCell ref="T8:V8"/>
+    <mergeCell ref="W8:Y8"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="T10:V10"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="V6:Y6"/>
+    <mergeCell ref="T15:V15"/>
+    <mergeCell ref="W15:Y15"/>
+    <mergeCell ref="T17:Y17"/>
+    <mergeCell ref="T18:Y18"/>
+    <mergeCell ref="W14:Y14"/>
+    <mergeCell ref="T14:V14"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="E1:Q1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="A26:B27"/>
+    <mergeCell ref="A15:B15"/>
   </mergeCells>
   <conditionalFormatting sqref="F52:F53">
     <cfRule type="expression" dxfId="53" priority="2" stopIfTrue="1">
@@ -25473,21 +25473,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001185193EED7D7C45B2181268987EEB31" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0398fff93780d69aa75df20e85be37f6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="55e0dd24fae28f1b5dd5f79afbe3cfeb">
     <xsd:element name="properties">
@@ -25601,10 +25586,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7243C670-E16E-4DBD-9932-9E3C368D5054}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5245AC5-DF56-430A-AECE-726FB05E2AD0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -25625,17 +25633,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5245AC5-DF56-430A-AECE-726FB05E2AD0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7243C670-E16E-4DBD-9932-9E3C368D5054}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>